<commit_message>
Added butterfly sheet to change spreadsheet
</commit_message>
<xml_diff>
--- a/change.xlsx
+++ b/change.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elinfalla/Dropbox/2020-21/_Imperial_MSc/_Project/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4C2D415-C975-1448-9283-22271A186BD6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{912841A1-83DA-B54F-94C0-171A8DEEF4B7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="2" xr2:uid="{D6098C0C-5D8D-4C8C-96C7-825309F64318}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="4" xr2:uid="{D6098C0C-5D8D-4C8C-96C7-825309F64318}"/>
   </bookViews>
   <sheets>
     <sheet name="pollinators" sheetId="1" r:id="rId1"/>
     <sheet name="pollinator_key" sheetId="2" r:id="rId2"/>
     <sheet name="mammals" sheetId="3" r:id="rId3"/>
     <sheet name="mammal_key" sheetId="5" r:id="rId4"/>
+    <sheet name="butterflies" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -3465,7 +3466,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="190">
   <si>
     <t>hay_sil</t>
   </si>
@@ -4110,6 +4111,18 @@
   <si>
     <t>Ai_yr1</t>
     <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>R_early</t>
+  </si>
+  <si>
+    <t>R_mid</t>
+  </si>
+  <si>
+    <t>R_late</t>
+  </si>
+  <si>
+    <t>R_damp plant</t>
   </si>
 </sst>
 </file>
@@ -4283,7 +4296,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -4300,11 +4313,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -4407,6 +4440,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4877,7 +4922,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R1" sqref="R1:AC1"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -6297,8 +6342,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B96CB725-FD77-4D87-887C-A852102D004E}">
   <dimension ref="A1:AS33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AP6" sqref="AP6"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -7315,4 +7360,232 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39D49925-3FF0-9342-AD81-24B91F515069}">
+  <dimension ref="A1:AY7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:51" ht="32">
+      <c r="A1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="43" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="43" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="43" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="43" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" s="44" t="s">
+        <v>93</v>
+      </c>
+      <c r="G1" s="45" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="45" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" s="45" t="s">
+        <v>30</v>
+      </c>
+      <c r="J1" s="45" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" s="45" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" s="45" t="s">
+        <v>27</v>
+      </c>
+      <c r="M1" s="45" t="s">
+        <v>26</v>
+      </c>
+      <c r="N1" s="45" t="s">
+        <v>25</v>
+      </c>
+      <c r="O1" s="45" t="s">
+        <v>24</v>
+      </c>
+      <c r="P1" s="45" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q1" s="45" t="s">
+        <v>22</v>
+      </c>
+      <c r="R1" s="45" t="s">
+        <v>21</v>
+      </c>
+      <c r="S1" s="45" t="s">
+        <v>186</v>
+      </c>
+      <c r="T1" s="45" t="s">
+        <v>187</v>
+      </c>
+      <c r="U1" s="45" t="s">
+        <v>188</v>
+      </c>
+      <c r="V1" s="45" t="s">
+        <v>8</v>
+      </c>
+      <c r="W1" s="45" t="s">
+        <v>7</v>
+      </c>
+      <c r="X1" s="45" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y1" s="45" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z1" s="45" t="s">
+        <v>189</v>
+      </c>
+      <c r="AA1" s="46"/>
+      <c r="AB1" s="45"/>
+      <c r="AC1" s="45"/>
+      <c r="AD1" s="45"/>
+      <c r="AE1" s="45"/>
+      <c r="AF1" s="45"/>
+      <c r="AG1" s="45"/>
+      <c r="AH1" s="45"/>
+      <c r="AI1" s="45"/>
+      <c r="AJ1" s="45"/>
+      <c r="AK1" s="45"/>
+      <c r="AL1" s="45"/>
+      <c r="AM1" s="45"/>
+      <c r="AN1" s="45"/>
+      <c r="AO1" s="45"/>
+      <c r="AP1" s="45"/>
+      <c r="AQ1" s="45"/>
+      <c r="AR1" s="45"/>
+      <c r="AS1" s="45"/>
+      <c r="AT1" s="45"/>
+      <c r="AU1" s="45"/>
+      <c r="AV1" s="45"/>
+      <c r="AW1" s="45"/>
+      <c r="AX1" s="45"/>
+      <c r="AY1" s="45"/>
+    </row>
+    <row r="2" spans="1:51" ht="16">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>-1</v>
+      </c>
+      <c r="O2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:51" ht="16">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <v>-1</v>
+      </c>
+      <c r="E3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:51" ht="16">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>-1</v>
+      </c>
+      <c r="H4">
+        <v>-1</v>
+      </c>
+      <c r="I4">
+        <v>-1</v>
+      </c>
+      <c r="J4">
+        <v>-1</v>
+      </c>
+      <c r="K4">
+        <v>-1</v>
+      </c>
+      <c r="L4">
+        <v>-1</v>
+      </c>
+      <c r="S4">
+        <v>-1</v>
+      </c>
+      <c r="T4">
+        <v>-1</v>
+      </c>
+      <c r="U4">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:51" ht="16">
+      <c r="A5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="S5">
+        <v>-1</v>
+      </c>
+      <c r="T5">
+        <v>-1</v>
+      </c>
+      <c r="U5">
+        <v>-1</v>
+      </c>
+      <c r="V5">
+        <v>-1</v>
+      </c>
+      <c r="W5">
+        <v>-1</v>
+      </c>
+      <c r="X5">
+        <v>-1</v>
+      </c>
+      <c r="Y5">
+        <v>-1</v>
+      </c>
+      <c r="Z5">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:51" ht="16">
+      <c r="A6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>-1</v>
+      </c>
+      <c r="P6">
+        <v>-1</v>
+      </c>
+      <c r="Q6">
+        <v>-1</v>
+      </c>
+      <c r="R6">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:51" ht="16">
+      <c r="A7" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="E7">
+        <v>-1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
change bee hab colnames to match butterfly, add inc_stocking butler change
</commit_message>
<xml_diff>
--- a/change.xlsx
+++ b/change.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elinfalla/Dropbox/2020-21/_Imperial_MSc/_Project/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{229A28FD-C07F-7447-A8E6-BEA00F3E5A9A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC05D367-5257-F34C-9115-D35C24EB3883}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="4" xr2:uid="{D6098C0C-5D8D-4C8C-96C7-825309F64318}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{D6098C0C-5D8D-4C8C-96C7-825309F64318}"/>
   </bookViews>
   <sheets>
     <sheet name="pollinators" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,6 @@
     <sheet name="butterflies" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -94,7 +93,7 @@
 In terms of your specific question – the answer is “it depends”. If the agricultural change results in both a loss of foraging habitat per se AND a loss of forage plants in the remaining foraging habitat (i.e. reduction in quality) then you would fill in both [cells D1 and N1]. If it results in a loss of foraging habitat but quality of remaining habitat is unaffected then you’d just mark-up the first [cell N1]. Hope that makes sense! How’s this project coming together – what are publication plans etc?</t>
       </text>
     </comment>
-    <comment ref="B2" authorId="1" shapeId="0" xr:uid="{12E63D2F-3418-456A-86CE-543FEF1ED90C}">
+    <comment ref="C2" authorId="1" shapeId="0" xr:uid="{12E63D2F-3418-456A-86CE-543FEF1ED90C}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -103,7 +102,7 @@
 This column gets a -1 if the change results in a reduction in forage plants in the hedge (i.e. a reduction in forage QUALITY, as opposed to a reduction in forage HABITAT).</t>
       </text>
     </comment>
-    <comment ref="C2" authorId="2" shapeId="0" xr:uid="{A5FFC6A3-8E1D-4D99-84D6-11453E436A7C}">
+    <comment ref="D2" authorId="2" shapeId="0" xr:uid="{A5FFC6A3-8E1D-4D99-84D6-11453E436A7C}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -112,7 +111,7 @@
 This column gets a -1 if the change results in a reduction in forage plants in the margin (i.e. a reduction in forage QUALITY, as opposed to a reduction in forage HABITAT).</t>
       </text>
     </comment>
-    <comment ref="D2" authorId="3" shapeId="0" xr:uid="{A4FA3B61-D780-4313-A275-F972791A3AD0}">
+    <comment ref="E2" authorId="3" shapeId="0" xr:uid="{A4FA3B61-D780-4313-A275-F972791A3AD0}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -121,7 +120,7 @@
 This column gets a -1 if the change results in a reduction in forage plants in the arable crop area (i.e. a reduction in forage QUALITY, as opposed to a reduction in forage HABITAT).</t>
       </text>
     </comment>
-    <comment ref="E2" authorId="4" shapeId="0" xr:uid="{DDE26C6C-5D60-45EC-8E7B-567092A4CCFE}">
+    <comment ref="F2" authorId="4" shapeId="0" xr:uid="{DDE26C6C-5D60-45EC-8E7B-567092A4CCFE}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -130,7 +129,7 @@
 This column gets a -1 if the change results in a reduction in forage plants in the grass field (i.e. a reduction in forage QUALITY, as opposed to a reduction in forage HABITAT).</t>
       </text>
     </comment>
-    <comment ref="F2" authorId="5" shapeId="0" xr:uid="{E85EAACE-3D6F-490A-A874-B78574BC3A18}">
+    <comment ref="I2" authorId="5" shapeId="0" xr:uid="{E85EAACE-3D6F-490A-A874-B78574BC3A18}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -138,7 +137,7 @@
     Hedge - early flight period</t>
       </text>
     </comment>
-    <comment ref="G2" authorId="6" shapeId="0" xr:uid="{E7DD46A6-F9D2-4082-B7FD-1C62A7012780}">
+    <comment ref="J2" authorId="6" shapeId="0" xr:uid="{E7DD46A6-F9D2-4082-B7FD-1C62A7012780}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -146,7 +145,7 @@
     Hedge - mid flight period</t>
       </text>
     </comment>
-    <comment ref="H2" authorId="7" shapeId="0" xr:uid="{93A93BB9-18C3-4473-8D44-E925AF1076FD}">
+    <comment ref="K2" authorId="7" shapeId="0" xr:uid="{93A93BB9-18C3-4473-8D44-E925AF1076FD}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -154,7 +153,7 @@
     Hedge - late flight period</t>
       </text>
     </comment>
-    <comment ref="I2" authorId="8" shapeId="0" xr:uid="{8FF21DDF-531B-4FCA-B3F6-FCA8674A96A7}">
+    <comment ref="L2" authorId="8" shapeId="0" xr:uid="{8FF21DDF-531B-4FCA-B3F6-FCA8674A96A7}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -162,7 +161,7 @@
     Margin - early flight period</t>
       </text>
     </comment>
-    <comment ref="J2" authorId="9" shapeId="0" xr:uid="{F8488B80-45A8-4869-8F4B-0AF68B71D35D}">
+    <comment ref="M2" authorId="9" shapeId="0" xr:uid="{F8488B80-45A8-4869-8F4B-0AF68B71D35D}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -170,7 +169,7 @@
     Margin - mid flight period</t>
       </text>
     </comment>
-    <comment ref="K2" authorId="10" shapeId="0" xr:uid="{A8F87931-1371-498C-A6F1-DD38B8ACE74D}">
+    <comment ref="N2" authorId="10" shapeId="0" xr:uid="{A8F87931-1371-498C-A6F1-DD38B8ACE74D}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -178,7 +177,7 @@
     Margin - late flight period</t>
       </text>
     </comment>
-    <comment ref="L2" authorId="11" shapeId="0" xr:uid="{BBDD0C84-AF5D-46EA-9C10-64A2D588C54F}">
+    <comment ref="O2" authorId="11" shapeId="0" xr:uid="{BBDD0C84-AF5D-46EA-9C10-64A2D588C54F}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -186,7 +185,7 @@
     Crop (arable) - early flight period</t>
       </text>
     </comment>
-    <comment ref="M2" authorId="12" shapeId="0" xr:uid="{A4ED52F3-90DC-4C64-B795-DBB2D853B8BC}">
+    <comment ref="P2" authorId="12" shapeId="0" xr:uid="{A4ED52F3-90DC-4C64-B795-DBB2D853B8BC}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -194,7 +193,7 @@
     Crop (arable) - mid flight period</t>
       </text>
     </comment>
-    <comment ref="N2" authorId="13" shapeId="0" xr:uid="{69B92BAE-B610-4F6E-BC37-BB85D80011AD}">
+    <comment ref="Q2" authorId="13" shapeId="0" xr:uid="{69B92BAE-B610-4F6E-BC37-BB85D80011AD}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -202,7 +201,7 @@
     Crop (arable) - late flight period</t>
       </text>
     </comment>
-    <comment ref="O2" authorId="14" shapeId="0" xr:uid="{819BF94A-B0FA-44CE-BFAE-328D48B2B389}">
+    <comment ref="R2" authorId="14" shapeId="0" xr:uid="{819BF94A-B0FA-44CE-BFAE-328D48B2B389}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -210,7 +209,7 @@
     Crop (grass) - early flight period</t>
       </text>
     </comment>
-    <comment ref="P2" authorId="15" shapeId="0" xr:uid="{A671B92F-735C-4E1B-8C51-41828B1B17EF}">
+    <comment ref="S2" authorId="15" shapeId="0" xr:uid="{A671B92F-735C-4E1B-8C51-41828B1B17EF}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -218,7 +217,7 @@
     Crop (grass) - mid flight period</t>
       </text>
     </comment>
-    <comment ref="Q2" authorId="16" shapeId="0" xr:uid="{A6DF340C-D9B4-4213-B8D0-BC13399B784F}">
+    <comment ref="T2" authorId="16" shapeId="0" xr:uid="{A6DF340C-D9B4-4213-B8D0-BC13399B784F}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -226,7 +225,7 @@
     Crop (grass) - late flight period</t>
       </text>
     </comment>
-    <comment ref="R2" authorId="17" shapeId="0" xr:uid="{C439AAA7-ACD4-4DF7-9B88-A19F61BEE251}">
+    <comment ref="W2" authorId="17" shapeId="0" xr:uid="{C439AAA7-ACD4-4DF7-9B88-A19F61BEE251}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -234,7 +233,7 @@
     Hedge nest</t>
       </text>
     </comment>
-    <comment ref="S2" authorId="18" shapeId="0" xr:uid="{4DEAFCB3-D3C5-467A-B77C-9D5987F93123}">
+    <comment ref="X2" authorId="18" shapeId="0" xr:uid="{4DEAFCB3-D3C5-467A-B77C-9D5987F93123}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -242,7 +241,7 @@
     Hedge nest</t>
       </text>
     </comment>
-    <comment ref="T2" authorId="19" shapeId="0" xr:uid="{751B814D-5DC3-49BB-998F-BF86DA7FC664}">
+    <comment ref="Y2" authorId="19" shapeId="0" xr:uid="{751B814D-5DC3-49BB-998F-BF86DA7FC664}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -250,7 +249,7 @@
     Hedge nest</t>
       </text>
     </comment>
-    <comment ref="U2" authorId="20" shapeId="0" xr:uid="{CE003D41-2E14-4AC4-A2B7-989C38B416B0}">
+    <comment ref="Z2" authorId="20" shapeId="0" xr:uid="{CE003D41-2E14-4AC4-A2B7-989C38B416B0}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -258,7 +257,7 @@
     Margin nest</t>
       </text>
     </comment>
-    <comment ref="V2" authorId="21" shapeId="0" xr:uid="{0D12942F-1149-41D9-9FCC-B574F659E0C5}">
+    <comment ref="AA2" authorId="21" shapeId="0" xr:uid="{0D12942F-1149-41D9-9FCC-B574F659E0C5}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -266,7 +265,7 @@
     Margin nest</t>
       </text>
     </comment>
-    <comment ref="W2" authorId="22" shapeId="0" xr:uid="{BF4C582D-E615-4D2B-8FA2-B3377ED3A651}">
+    <comment ref="AB2" authorId="22" shapeId="0" xr:uid="{BF4C582D-E615-4D2B-8FA2-B3377ED3A651}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -274,7 +273,7 @@
     Margin nest</t>
       </text>
     </comment>
-    <comment ref="X2" authorId="23" shapeId="0" xr:uid="{577817A3-41CF-4B09-B701-1DA64D94A3F7}">
+    <comment ref="AC2" authorId="23" shapeId="0" xr:uid="{577817A3-41CF-4B09-B701-1DA64D94A3F7}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -282,7 +281,7 @@
     Margin nest</t>
       </text>
     </comment>
-    <comment ref="Y2" authorId="24" shapeId="0" xr:uid="{61328AAB-8080-40A5-BB72-DE3F063064D6}">
+    <comment ref="AD2" authorId="24" shapeId="0" xr:uid="{61328AAB-8080-40A5-BB72-DE3F063064D6}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -290,7 +289,7 @@
     Crop (arable) nest</t>
       </text>
     </comment>
-    <comment ref="Z2" authorId="25" shapeId="0" xr:uid="{08D8BC3C-7DE2-46DE-A501-79F9B77FC5A6}">
+    <comment ref="AE2" authorId="25" shapeId="0" xr:uid="{08D8BC3C-7DE2-46DE-A501-79F9B77FC5A6}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -298,7 +297,7 @@
     Crop (grass) nest</t>
       </text>
     </comment>
-    <comment ref="AA2" authorId="26" shapeId="0" xr:uid="{60F49050-15F0-4A01-B60D-D08CFC1500EA}">
+    <comment ref="AF2" authorId="26" shapeId="0" xr:uid="{60F49050-15F0-4A01-B60D-D08CFC1500EA}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -306,7 +305,7 @@
     Crop (grass) nest</t>
       </text>
     </comment>
-    <comment ref="AB2" authorId="27" shapeId="0" xr:uid="{53B38088-2842-4886-AD04-FB278DF6E6D5}">
+    <comment ref="AG2" authorId="27" shapeId="0" xr:uid="{53B38088-2842-4886-AD04-FB278DF6E6D5}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -314,7 +313,7 @@
     Crop (grass) nest</t>
       </text>
     </comment>
-    <comment ref="AC2" authorId="28" shapeId="0" xr:uid="{E625A537-1514-4930-ADE3-685B712C12DD}">
+    <comment ref="AH2" authorId="28" shapeId="0" xr:uid="{E625A537-1514-4930-ADE3-685B712C12DD}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -322,7 +321,7 @@
     Crop (grass) nest</t>
       </text>
     </comment>
-    <comment ref="AD2" authorId="29" shapeId="0" xr:uid="{2B82472E-59FF-4148-AB12-C02672624F2E}">
+    <comment ref="AK2" authorId="29" shapeId="0" xr:uid="{2B82472E-59FF-4148-AB12-C02672624F2E}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -330,7 +329,7 @@
     Hedge - plants associated with damp areas specifically</t>
       </text>
     </comment>
-    <comment ref="AE2" authorId="30" shapeId="0" xr:uid="{74099FC7-8ABC-4BCA-B048-586D8C2AB079}">
+    <comment ref="AL2" authorId="30" shapeId="0" xr:uid="{74099FC7-8ABC-4BCA-B048-586D8C2AB079}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -338,7 +337,7 @@
     Margin - plants associated with damp areas specifically</t>
       </text>
     </comment>
-    <comment ref="AF2" authorId="31" shapeId="0" xr:uid="{48C3A0E7-35F7-49D1-B02F-BFD8904E48CB}">
+    <comment ref="AM2" authorId="31" shapeId="0" xr:uid="{48C3A0E7-35F7-49D1-B02F-BFD8904E48CB}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -346,7 +345,7 @@
     Crop (arable) - plants associated with damp areas specifically</t>
       </text>
     </comment>
-    <comment ref="AG2" authorId="32" shapeId="0" xr:uid="{90E5597C-0F3C-4878-B496-32CD19452B20}">
+    <comment ref="AN2" authorId="32" shapeId="0" xr:uid="{90E5597C-0F3C-4878-B496-32CD19452B20}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -354,7 +353,7 @@
     Crop (grass) - plants associated with damp areas specifically</t>
       </text>
     </comment>
-    <comment ref="D3" authorId="33" shapeId="0" xr:uid="{C1BDF87D-1D41-44ED-9DB5-82CE7A80DFFC}">
+    <comment ref="E3" authorId="33" shapeId="0" xr:uid="{C1BDF87D-1D41-44ED-9DB5-82CE7A80DFFC}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -386,7 +385,7 @@
     ww to spring linseed</t>
       </text>
     </comment>
-    <comment ref="D13" authorId="37" shapeId="0" xr:uid="{48C6BB13-E6DC-42AB-B35A-0607696151B4}">
+    <comment ref="E13" authorId="37" shapeId="0" xr:uid="{48C6BB13-E6DC-42AB-B35A-0607696151B4}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -394,7 +393,7 @@
     spring linseed is a flowering crop, and less chemicals are used on it (ABC 2019)</t>
       </text>
     </comment>
-    <comment ref="M13" authorId="38" shapeId="0" xr:uid="{7435BEBC-43A5-4387-A373-041298C99067}">
+    <comment ref="P13" authorId="38" shapeId="0" xr:uid="{7435BEBC-43A5-4387-A373-041298C99067}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -412,7 +411,7 @@
     ww to spring beans</t>
       </text>
     </comment>
-    <comment ref="D14" authorId="40" shapeId="0" xr:uid="{6B5EBF82-CF92-4DE1-87B1-3D2CA880033A}">
+    <comment ref="E14" authorId="40" shapeId="0" xr:uid="{6B5EBF82-CF92-4DE1-87B1-3D2CA880033A}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -420,7 +419,7 @@
     beans are a flowering crop, plus crop protection for beans is lower (ww = £240/ha, sprbean = £125/ha, ABC 2019)</t>
       </text>
     </comment>
-    <comment ref="L14" authorId="41" shapeId="0" xr:uid="{1C676EBF-A20E-40B0-8CCD-00E3E4D6F477}">
+    <comment ref="O14" authorId="41" shapeId="0" xr:uid="{1C676EBF-A20E-40B0-8CCD-00E3E4D6F477}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -454,7 +453,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D32" authorId="42" shapeId="0" xr:uid="{53D826E0-66F7-499A-B98C-7553566BEBF8}">
+    <comment ref="E32" authorId="42" shapeId="0" xr:uid="{53D826E0-66F7-499A-B98C-7553566BEBF8}">
       <text>
         <r>
           <rPr>
@@ -480,7 +479,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M32" authorId="42" shapeId="0" xr:uid="{9379C0D0-F70C-4E8D-9859-3C451B3E0ED8}">
+    <comment ref="P32" authorId="42" shapeId="0" xr:uid="{9379C0D0-F70C-4E8D-9859-3C451B3E0ED8}">
       <text>
         <r>
           <rPr>
@@ -508,7 +507,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D34" authorId="42" shapeId="0" xr:uid="{D04462C5-36F9-4A51-BC01-8C5A7D6C54BE}">
+    <comment ref="E34" authorId="42" shapeId="0" xr:uid="{D04462C5-36F9-4A51-BC01-8C5A7D6C54BE}">
       <text>
         <r>
           <rPr>
@@ -534,7 +533,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L34" authorId="42" shapeId="0" xr:uid="{A4D197B3-AFE2-4A27-9C2D-6B9A38C3C2F7}">
+    <comment ref="O34" authorId="42" shapeId="0" xr:uid="{A4D197B3-AFE2-4A27-9C2D-6B9A38C3C2F7}">
       <text>
         <r>
           <rPr>
@@ -560,7 +559,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D36" authorId="42" shapeId="0" xr:uid="{E3B2C3A2-A046-4882-878A-069572F69AC4}">
+    <comment ref="E36" authorId="42" shapeId="0" xr:uid="{E3B2C3A2-A046-4882-878A-069572F69AC4}">
       <text>
         <r>
           <rPr>
@@ -587,7 +586,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L36" authorId="42" shapeId="0" xr:uid="{9B21C236-1544-4B60-9206-D9E0113704A7}">
+    <comment ref="O36" authorId="42" shapeId="0" xr:uid="{9B21C236-1544-4B60-9206-D9E0113704A7}">
       <text>
         <r>
           <rPr>
@@ -614,7 +613,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D38" authorId="42" shapeId="0" xr:uid="{DD7709C3-AECD-4ABC-B2B1-205AD08272FF}">
+    <comment ref="E38" authorId="42" shapeId="0" xr:uid="{DD7709C3-AECD-4ABC-B2B1-205AD08272FF}">
       <text>
         <r>
           <rPr>
@@ -640,7 +639,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D41" authorId="42" shapeId="0" xr:uid="{47DE150F-B54E-4A17-A4AD-B1DCBA39F1F0}">
+    <comment ref="E41" authorId="42" shapeId="0" xr:uid="{47DE150F-B54E-4A17-A4AD-B1DCBA39F1F0}">
       <text>
         <r>
           <rPr>
@@ -666,7 +665,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L41" authorId="42" shapeId="0" xr:uid="{9BEA5C6D-42A6-4447-8698-5F89FCB7CC48}">
+    <comment ref="O41" authorId="42" shapeId="0" xr:uid="{9BEA5C6D-42A6-4447-8698-5F89FCB7CC48}">
       <text>
         <r>
           <rPr>
@@ -692,7 +691,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M41" authorId="42" shapeId="0" xr:uid="{950FB1BA-08C6-481A-BAA1-87123CBB9FC5}">
+    <comment ref="P41" authorId="42" shapeId="0" xr:uid="{950FB1BA-08C6-481A-BAA1-87123CBB9FC5}">
       <text>
         <r>
           <rPr>
@@ -720,7 +719,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D43" authorId="42" shapeId="0" xr:uid="{F4391AC5-316D-4971-9DE0-03C289742049}">
+    <comment ref="E43" authorId="42" shapeId="0" xr:uid="{F4391AC5-316D-4971-9DE0-03C289742049}">
       <text>
         <r>
           <rPr>
@@ -746,7 +745,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L43" authorId="42" shapeId="0" xr:uid="{4B5C19F6-BE09-490B-AF49-9C714538AC29}">
+    <comment ref="O43" authorId="42" shapeId="0" xr:uid="{4B5C19F6-BE09-490B-AF49-9C714538AC29}">
       <text>
         <r>
           <rPr>
@@ -772,7 +771,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D44" authorId="42" shapeId="0" xr:uid="{0B926EFC-4F27-449B-8C57-7B25F6CF46C9}">
+    <comment ref="E44" authorId="42" shapeId="0" xr:uid="{0B926EFC-4F27-449B-8C57-7B25F6CF46C9}">
       <text>
         <r>
           <rPr>
@@ -799,7 +798,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L44" authorId="42" shapeId="0" xr:uid="{FF5D0C02-4398-415B-B19C-19526E678D06}">
+    <comment ref="O44" authorId="42" shapeId="0" xr:uid="{FF5D0C02-4398-415B-B19C-19526E678D06}">
       <text>
         <r>
           <rPr>
@@ -826,7 +825,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D45" authorId="42" shapeId="0" xr:uid="{105495CB-88D0-4F30-8DD5-ACFDA27F7107}">
+    <comment ref="E45" authorId="42" shapeId="0" xr:uid="{105495CB-88D0-4F30-8DD5-ACFDA27F7107}">
       <text>
         <r>
           <rPr>
@@ -852,7 +851,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D46" authorId="42" shapeId="0" xr:uid="{7F528817-12BF-4081-9C72-8C01AB24FA9B}">
+    <comment ref="E46" authorId="42" shapeId="0" xr:uid="{7F528817-12BF-4081-9C72-8C01AB24FA9B}">
       <text>
         <r>
           <rPr>
@@ -879,7 +878,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L46" authorId="42" shapeId="0" xr:uid="{701FA78D-EAD8-4D73-9550-381BD875E87E}">
+    <comment ref="O46" authorId="42" shapeId="0" xr:uid="{701FA78D-EAD8-4D73-9550-381BD875E87E}">
       <text>
         <r>
           <rPr>
@@ -906,7 +905,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D47" authorId="42" shapeId="0" xr:uid="{3CD6C769-FB14-4111-B02E-940E6DEDACFD}">
+    <comment ref="E47" authorId="42" shapeId="0" xr:uid="{3CD6C769-FB14-4111-B02E-940E6DEDACFD}">
       <text>
         <r>
           <rPr>
@@ -933,7 +932,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L47" authorId="42" shapeId="0" xr:uid="{1F8B46C9-B546-4480-9864-EBAFDDF26FA9}">
+    <comment ref="O47" authorId="42" shapeId="0" xr:uid="{1F8B46C9-B546-4480-9864-EBAFDDF26FA9}">
       <text>
         <r>
           <rPr>
@@ -987,7 +986,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D49" authorId="42" shapeId="0" xr:uid="{1C118D62-65EF-4C11-B37B-F048AEAE7DFD}">
+    <comment ref="E49" authorId="42" shapeId="0" xr:uid="{1C118D62-65EF-4C11-B37B-F048AEAE7DFD}">
       <text>
         <r>
           <rPr>
@@ -1014,7 +1013,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L49" authorId="42" shapeId="0" xr:uid="{2AFDF31F-2C75-4E84-A8AF-643F640FECB1}">
+    <comment ref="O49" authorId="42" shapeId="0" xr:uid="{2AFDF31F-2C75-4E84-A8AF-643F640FECB1}">
       <text>
         <r>
           <rPr>
@@ -1041,7 +1040,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D50" authorId="42" shapeId="0" xr:uid="{8BC0A7A5-3903-4588-ADC6-E8A98688DF52}">
+    <comment ref="E50" authorId="42" shapeId="0" xr:uid="{8BC0A7A5-3903-4588-ADC6-E8A98688DF52}">
       <text>
         <r>
           <rPr>
@@ -1068,7 +1067,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L50" authorId="42" shapeId="0" xr:uid="{5E5343BD-BDC9-4266-B66E-D1A09D638F99}">
+    <comment ref="O50" authorId="42" shapeId="0" xr:uid="{5E5343BD-BDC9-4266-B66E-D1A09D638F99}">
       <text>
         <r>
           <rPr>
@@ -1095,7 +1094,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D52" authorId="42" shapeId="0" xr:uid="{189CD8CC-E5E1-416E-952D-4B405A09D533}">
+    <comment ref="E52" authorId="42" shapeId="0" xr:uid="{189CD8CC-E5E1-416E-952D-4B405A09D533}">
       <text>
         <r>
           <rPr>
@@ -1122,7 +1121,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L52" authorId="42" shapeId="0" xr:uid="{6338A60A-D3B7-40A0-9512-DBB95C547564}">
+    <comment ref="O52" authorId="42" shapeId="0" xr:uid="{6338A60A-D3B7-40A0-9512-DBB95C547564}">
       <text>
         <r>
           <rPr>
@@ -1148,7 +1147,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D53" authorId="42" shapeId="0" xr:uid="{AF176DAC-4BFD-4240-9F0E-83F7D2B9370D}">
+    <comment ref="E53" authorId="42" shapeId="0" xr:uid="{AF176DAC-4BFD-4240-9F0E-83F7D2B9370D}">
       <text>
         <r>
           <rPr>
@@ -1175,7 +1174,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L53" authorId="42" shapeId="0" xr:uid="{6C28AC3E-E506-4D18-83BB-2618692CCDF1}">
+    <comment ref="O53" authorId="42" shapeId="0" xr:uid="{6C28AC3E-E506-4D18-83BB-2618692CCDF1}">
       <text>
         <r>
           <rPr>
@@ -1201,7 +1200,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D56" authorId="42" shapeId="0" xr:uid="{B900B5DA-939E-4FB6-8AE8-FAF3441715C8}">
+    <comment ref="E56" authorId="42" shapeId="0" xr:uid="{B900B5DA-939E-4FB6-8AE8-FAF3441715C8}">
       <text>
         <r>
           <rPr>
@@ -1228,7 +1227,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L56" authorId="42" shapeId="0" xr:uid="{8D07C60C-9F9A-43D4-A524-114CAD7670A0}">
+    <comment ref="O56" authorId="42" shapeId="0" xr:uid="{8D07C60C-9F9A-43D4-A524-114CAD7670A0}">
       <text>
         <r>
           <rPr>
@@ -1254,7 +1253,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D59" authorId="42" shapeId="0" xr:uid="{F9FBC64A-6FD5-4E69-B90C-34792F9576E2}">
+    <comment ref="E59" authorId="42" shapeId="0" xr:uid="{F9FBC64A-6FD5-4E69-B90C-34792F9576E2}">
       <text>
         <r>
           <rPr>
@@ -1281,7 +1280,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L59" authorId="42" shapeId="0" xr:uid="{02119076-93E1-4745-A7C9-CDAEF337C3D2}">
+    <comment ref="O59" authorId="42" shapeId="0" xr:uid="{02119076-93E1-4745-A7C9-CDAEF337C3D2}">
       <text>
         <r>
           <rPr>
@@ -1333,7 +1332,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D65" authorId="42" shapeId="0" xr:uid="{AE3CF127-6011-4F46-A9F1-C9E08E2FD3F4}">
+    <comment ref="E65" authorId="42" shapeId="0" xr:uid="{AE3CF127-6011-4F46-A9F1-C9E08E2FD3F4}">
       <text>
         <r>
           <rPr>
@@ -1359,7 +1358,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M65" authorId="42" shapeId="0" xr:uid="{C582120E-4979-49EF-8D89-712834B9A051}">
+    <comment ref="P65" authorId="42" shapeId="0" xr:uid="{C582120E-4979-49EF-8D89-712834B9A051}">
       <text>
         <r>
           <rPr>
@@ -1387,7 +1386,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D66" authorId="42" shapeId="0" xr:uid="{33961048-D789-4FB7-B4A4-0E1A42CBBBA6}">
+    <comment ref="E66" authorId="42" shapeId="0" xr:uid="{33961048-D789-4FB7-B4A4-0E1A42CBBBA6}">
       <text>
         <r>
           <rPr>
@@ -1413,7 +1412,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L66" authorId="42" shapeId="0" xr:uid="{EBAC13E1-E1C8-4B02-BDD4-DD5097AFA28D}">
+    <comment ref="O66" authorId="42" shapeId="0" xr:uid="{EBAC13E1-E1C8-4B02-BDD4-DD5097AFA28D}">
       <text>
         <r>
           <rPr>
@@ -1439,7 +1438,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D67" authorId="42" shapeId="0" xr:uid="{80C56F53-5D92-486C-9AB1-B86F91F7F99F}">
+    <comment ref="E67" authorId="42" shapeId="0" xr:uid="{80C56F53-5D92-486C-9AB1-B86F91F7F99F}">
       <text>
         <r>
           <rPr>
@@ -1466,7 +1465,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L67" authorId="42" shapeId="0" xr:uid="{CFFB8458-A892-422B-B95A-F0E5C0A45E5A}">
+    <comment ref="O67" authorId="42" shapeId="0" xr:uid="{CFFB8458-A892-422B-B95A-F0E5C0A45E5A}">
       <text>
         <r>
           <rPr>
@@ -1493,7 +1492,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D68" authorId="42" shapeId="0" xr:uid="{E4AD4F04-A558-4B06-9B19-C435A71FDD38}">
+    <comment ref="E68" authorId="42" shapeId="0" xr:uid="{E4AD4F04-A558-4B06-9B19-C435A71FDD38}">
       <text>
         <r>
           <rPr>
@@ -1519,7 +1518,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D70" authorId="42" shapeId="0" xr:uid="{D75567D0-02E5-4E48-92AD-65CB55A2DC92}">
+    <comment ref="E70" authorId="42" shapeId="0" xr:uid="{D75567D0-02E5-4E48-92AD-65CB55A2DC92}">
       <text>
         <r>
           <rPr>
@@ -1545,7 +1544,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L70" authorId="42" shapeId="0" xr:uid="{674F7976-F8A3-4579-8A54-9AC16F09EAEB}">
+    <comment ref="O70" authorId="42" shapeId="0" xr:uid="{674F7976-F8A3-4579-8A54-9AC16F09EAEB}">
       <text>
         <r>
           <rPr>
@@ -1571,7 +1570,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M70" authorId="42" shapeId="0" xr:uid="{D2E71D98-DFB1-4618-BE8A-C9FF92FF647C}">
+    <comment ref="P70" authorId="42" shapeId="0" xr:uid="{D2E71D98-DFB1-4618-BE8A-C9FF92FF647C}">
       <text>
         <r>
           <rPr>
@@ -1599,7 +1598,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D72" authorId="42" shapeId="0" xr:uid="{C117F31D-5517-4C8F-BBD0-403408D4C231}">
+    <comment ref="E72" authorId="42" shapeId="0" xr:uid="{C117F31D-5517-4C8F-BBD0-403408D4C231}">
       <text>
         <r>
           <rPr>
@@ -1625,7 +1624,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L72" authorId="42" shapeId="0" xr:uid="{5E704C8C-FCC6-4EED-94F2-5FBB01BF51E6}">
+    <comment ref="O72" authorId="42" shapeId="0" xr:uid="{5E704C8C-FCC6-4EED-94F2-5FBB01BF51E6}">
       <text>
         <r>
           <rPr>
@@ -1651,7 +1650,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D73" authorId="42" shapeId="0" xr:uid="{05B9E780-929C-46CD-8EF3-287D6684F03E}">
+    <comment ref="E73" authorId="42" shapeId="0" xr:uid="{05B9E780-929C-46CD-8EF3-287D6684F03E}">
       <text>
         <r>
           <rPr>
@@ -1678,7 +1677,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L73" authorId="42" shapeId="0" xr:uid="{9A9A6B1A-D0BF-428D-86C2-33F2777FDA7A}">
+    <comment ref="O73" authorId="42" shapeId="0" xr:uid="{9A9A6B1A-D0BF-428D-86C2-33F2777FDA7A}">
       <text>
         <r>
           <rPr>
@@ -1705,7 +1704,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D74" authorId="42" shapeId="0" xr:uid="{EB329E91-93E4-4466-9117-FE798238B495}">
+    <comment ref="E74" authorId="42" shapeId="0" xr:uid="{EB329E91-93E4-4466-9117-FE798238B495}">
       <text>
         <r>
           <rPr>
@@ -1731,7 +1730,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D75" authorId="42" shapeId="0" xr:uid="{3E963013-CF41-4CAB-A8AE-A3402CA38481}">
+    <comment ref="E75" authorId="42" shapeId="0" xr:uid="{3E963013-CF41-4CAB-A8AE-A3402CA38481}">
       <text>
         <r>
           <rPr>
@@ -1758,7 +1757,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L75" authorId="42" shapeId="0" xr:uid="{FDC08721-9055-4CED-8545-252A067D662A}">
+    <comment ref="O75" authorId="42" shapeId="0" xr:uid="{FDC08721-9055-4CED-8545-252A067D662A}">
       <text>
         <r>
           <rPr>
@@ -1785,7 +1784,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D76" authorId="42" shapeId="0" xr:uid="{1C793E1B-CF57-4232-A407-4CB7F7A60931}">
+    <comment ref="E76" authorId="42" shapeId="0" xr:uid="{1C793E1B-CF57-4232-A407-4CB7F7A60931}">
       <text>
         <r>
           <rPr>
@@ -1812,7 +1811,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L76" authorId="42" shapeId="0" xr:uid="{6387D793-B128-4B8D-A2EF-3F0202BCD448}">
+    <comment ref="O76" authorId="42" shapeId="0" xr:uid="{6387D793-B128-4B8D-A2EF-3F0202BCD448}">
       <text>
         <r>
           <rPr>
@@ -1866,7 +1865,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D78" authorId="42" shapeId="0" xr:uid="{B3F34FDD-2764-4C1D-B824-7442AB8A18EF}">
+    <comment ref="E78" authorId="42" shapeId="0" xr:uid="{B3F34FDD-2764-4C1D-B824-7442AB8A18EF}">
       <text>
         <r>
           <rPr>
@@ -1893,7 +1892,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L78" authorId="42" shapeId="0" xr:uid="{2ACFDB7E-49A6-44C2-9D31-93C06D34C406}">
+    <comment ref="O78" authorId="42" shapeId="0" xr:uid="{2ACFDB7E-49A6-44C2-9D31-93C06D34C406}">
       <text>
         <r>
           <rPr>
@@ -1920,7 +1919,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D79" authorId="42" shapeId="0" xr:uid="{8B3C6A25-AACF-4D15-9632-3820C06BA909}">
+    <comment ref="E79" authorId="42" shapeId="0" xr:uid="{8B3C6A25-AACF-4D15-9632-3820C06BA909}">
       <text>
         <r>
           <rPr>
@@ -1947,7 +1946,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L79" authorId="42" shapeId="0" xr:uid="{F061DCD5-9E44-4A39-9E90-9D128519E97B}">
+    <comment ref="O79" authorId="42" shapeId="0" xr:uid="{F061DCD5-9E44-4A39-9E90-9D128519E97B}">
       <text>
         <r>
           <rPr>
@@ -1974,7 +1973,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D81" authorId="42" shapeId="0" xr:uid="{6B5601C8-A674-4AC2-9EE4-E960F2FFE6A5}">
+    <comment ref="E81" authorId="42" shapeId="0" xr:uid="{6B5601C8-A674-4AC2-9EE4-E960F2FFE6A5}">
       <text>
         <r>
           <rPr>
@@ -2001,7 +2000,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L81" authorId="42" shapeId="0" xr:uid="{EEAD24E4-F042-436F-AB65-E6BC8F49C602}">
+    <comment ref="O81" authorId="42" shapeId="0" xr:uid="{EEAD24E4-F042-436F-AB65-E6BC8F49C602}">
       <text>
         <r>
           <rPr>
@@ -2027,7 +2026,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D82" authorId="42" shapeId="0" xr:uid="{0E4638AD-B72D-4DAD-A116-C12996000DD6}">
+    <comment ref="E82" authorId="42" shapeId="0" xr:uid="{0E4638AD-B72D-4DAD-A116-C12996000DD6}">
       <text>
         <r>
           <rPr>
@@ -2054,7 +2053,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L82" authorId="42" shapeId="0" xr:uid="{F2EC6289-B92A-4E32-AD2F-6595D31EBA48}">
+    <comment ref="O82" authorId="42" shapeId="0" xr:uid="{F2EC6289-B92A-4E32-AD2F-6595D31EBA48}">
       <text>
         <r>
           <rPr>
@@ -2080,7 +2079,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D85" authorId="42" shapeId="0" xr:uid="{E6A09427-297C-4EDB-B309-263E2E14B3B9}">
+    <comment ref="E85" authorId="42" shapeId="0" xr:uid="{E6A09427-297C-4EDB-B309-263E2E14B3B9}">
       <text>
         <r>
           <rPr>
@@ -2107,7 +2106,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L85" authorId="42" shapeId="0" xr:uid="{D44680CE-0E6A-4159-9C50-2EEBF6BF57F2}">
+    <comment ref="O85" authorId="42" shapeId="0" xr:uid="{D44680CE-0E6A-4159-9C50-2EEBF6BF57F2}">
       <text>
         <r>
           <rPr>
@@ -2133,7 +2132,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D88" authorId="42" shapeId="0" xr:uid="{0A868D5F-FA86-4372-AAC6-4160A4596BFB}">
+    <comment ref="E88" authorId="42" shapeId="0" xr:uid="{0A868D5F-FA86-4372-AAC6-4160A4596BFB}">
       <text>
         <r>
           <rPr>
@@ -2160,7 +2159,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L88" authorId="42" shapeId="0" xr:uid="{64086BDE-B297-43B9-B972-1277935023D1}">
+    <comment ref="O88" authorId="42" shapeId="0" xr:uid="{64086BDE-B297-43B9-B972-1277935023D1}">
       <text>
         <r>
           <rPr>
@@ -3467,7 +3466,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="199">
   <si>
     <t>hay_sil</t>
   </si>
@@ -3566,18 +3565,6 @@
   </si>
   <si>
     <t>H_early</t>
-  </si>
-  <si>
-    <t>CG_fhab</t>
-  </si>
-  <si>
-    <t>CA_fhab</t>
-  </si>
-  <si>
-    <t>M_fhab</t>
-  </si>
-  <si>
-    <t>H_fhab</t>
   </si>
   <si>
     <t>agric_change</t>
@@ -4154,6 +4141,15 @@
   </si>
   <si>
     <t>damp_end</t>
+  </si>
+  <si>
+    <t>nest_start</t>
+  </si>
+  <si>
+    <t>nest_end</t>
+  </si>
+  <si>
+    <t>inc_stocking</t>
   </si>
 </sst>
 </file>
@@ -4374,7 +4370,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -4500,6 +4496,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4831,107 +4837,107 @@
     <text>Notes:
 In terms of your specific question – the answer is “it depends”. If the agricultural change results in both a loss of foraging habitat per se AND a loss of forage plants in the remaining foraging habitat (i.e. reduction in quality) then you would fill in both [cells D1 and N1]. If it results in a loss of foraging habitat but quality of remaining habitat is unaffected then you’d just mark-up the first [cell N1]. Hope that makes sense! How’s this project coming together – what are publication plans etc?</text>
   </threadedComment>
-  <threadedComment ref="B2" dT="2020-06-17T09:40:57.59" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{12E63D2F-3418-456A-86CE-543FEF1ED90C}">
+  <threadedComment ref="C2" dT="2020-06-17T09:40:57.59" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{12E63D2F-3418-456A-86CE-543FEF1ED90C}">
     <text>Forages in hedge.
 This column gets a -1 if the change results in a reduction in forage plants in the hedge (i.e. a reduction in forage QUALITY, as opposed to a reduction in forage HABITAT).</text>
   </threadedComment>
-  <threadedComment ref="C2" dT="2020-06-17T09:41:04.61" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{A5FFC6A3-8E1D-4D99-84D6-11453E436A7C}">
+  <threadedComment ref="D2" dT="2020-06-17T09:41:04.61" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{A5FFC6A3-8E1D-4D99-84D6-11453E436A7C}">
     <text>Forages in margin.
 This column gets a -1 if the change results in a reduction in forage plants in the margin (i.e. a reduction in forage QUALITY, as opposed to a reduction in forage HABITAT).</text>
   </threadedComment>
-  <threadedComment ref="D2" dT="2020-06-17T09:41:13.38" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{A4FA3B61-D780-4313-A275-F972791A3AD0}">
+  <threadedComment ref="E2" dT="2020-06-17T09:41:13.38" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{A4FA3B61-D780-4313-A275-F972791A3AD0}">
     <text>Forages in crop (arable).
 This column gets a -1 if the change results in a reduction in forage plants in the arable crop area (i.e. a reduction in forage QUALITY, as opposed to a reduction in forage HABITAT).</text>
   </threadedComment>
-  <threadedComment ref="E2" dT="2020-06-17T09:41:19.91" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{DDE26C6C-5D60-45EC-8E7B-567092A4CCFE}">
+  <threadedComment ref="F2" dT="2020-06-17T09:41:19.91" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{DDE26C6C-5D60-45EC-8E7B-567092A4CCFE}">
     <text>Forages in crop (grass).
 This column gets a -1 if the change results in a reduction in forage plants in the grass field (i.e. a reduction in forage QUALITY, as opposed to a reduction in forage HABITAT).</text>
   </threadedComment>
-  <threadedComment ref="F2" dT="2020-06-17T09:42:12.45" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{E85EAACE-3D6F-490A-A874-B78574BC3A18}">
+  <threadedComment ref="I2" dT="2020-06-17T09:42:12.45" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{E85EAACE-3D6F-490A-A874-B78574BC3A18}">
     <text>Hedge - early flight period</text>
   </threadedComment>
-  <threadedComment ref="G2" dT="2020-06-17T09:45:53.90" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{E7DD46A6-F9D2-4082-B7FD-1C62A7012780}">
+  <threadedComment ref="J2" dT="2020-06-17T09:45:53.90" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{E7DD46A6-F9D2-4082-B7FD-1C62A7012780}">
     <text>Hedge - mid flight period</text>
   </threadedComment>
-  <threadedComment ref="H2" dT="2020-06-17T09:46:04.63" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{93A93BB9-18C3-4473-8D44-E925AF1076FD}">
+  <threadedComment ref="K2" dT="2020-06-17T09:46:04.63" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{93A93BB9-18C3-4473-8D44-E925AF1076FD}">
     <text>Hedge - late flight period</text>
   </threadedComment>
-  <threadedComment ref="I2" dT="2020-06-17T09:46:15.78" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{8FF21DDF-531B-4FCA-B3F6-FCA8674A96A7}">
+  <threadedComment ref="L2" dT="2020-06-17T09:46:15.78" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{8FF21DDF-531B-4FCA-B3F6-FCA8674A96A7}">
     <text>Margin - early flight period</text>
   </threadedComment>
-  <threadedComment ref="J2" dT="2020-06-17T09:46:23.71" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{F8488B80-45A8-4869-8F4B-0AF68B71D35D}">
+  <threadedComment ref="M2" dT="2020-06-17T09:46:23.71" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{F8488B80-45A8-4869-8F4B-0AF68B71D35D}">
     <text>Margin - mid flight period</text>
   </threadedComment>
-  <threadedComment ref="K2" dT="2020-06-17T09:46:31.44" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{A8F87931-1371-498C-A6F1-DD38B8ACE74D}">
+  <threadedComment ref="N2" dT="2020-06-17T09:46:31.44" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{A8F87931-1371-498C-A6F1-DD38B8ACE74D}">
     <text>Margin - late flight period</text>
   </threadedComment>
-  <threadedComment ref="L2" dT="2020-06-17T10:26:27.87" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{BBDD0C84-AF5D-46EA-9C10-64A2D588C54F}">
+  <threadedComment ref="O2" dT="2020-06-17T10:26:27.87" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{BBDD0C84-AF5D-46EA-9C10-64A2D588C54F}">
     <text>Crop (arable) - early flight period</text>
   </threadedComment>
-  <threadedComment ref="M2" dT="2020-06-17T10:26:36.17" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{A4ED52F3-90DC-4C64-B795-DBB2D853B8BC}">
+  <threadedComment ref="P2" dT="2020-06-17T10:26:36.17" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{A4ED52F3-90DC-4C64-B795-DBB2D853B8BC}">
     <text>Crop (arable) - mid flight period</text>
   </threadedComment>
-  <threadedComment ref="N2" dT="2020-06-17T10:26:48.29" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{69B92BAE-B610-4F6E-BC37-BB85D80011AD}">
+  <threadedComment ref="Q2" dT="2020-06-17T10:26:48.29" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{69B92BAE-B610-4F6E-BC37-BB85D80011AD}">
     <text>Crop (arable) - late flight period</text>
   </threadedComment>
-  <threadedComment ref="O2" dT="2020-06-17T10:26:56.53" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{819BF94A-B0FA-44CE-BFAE-328D48B2B389}">
+  <threadedComment ref="R2" dT="2020-06-17T10:26:56.53" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{819BF94A-B0FA-44CE-BFAE-328D48B2B389}">
     <text>Crop (grass) - early flight period</text>
   </threadedComment>
-  <threadedComment ref="P2" dT="2020-06-17T10:27:03.24" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{A671B92F-735C-4E1B-8C51-41828B1B17EF}">
+  <threadedComment ref="S2" dT="2020-06-17T10:27:03.24" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{A671B92F-735C-4E1B-8C51-41828B1B17EF}">
     <text>Crop (grass) - mid flight period</text>
   </threadedComment>
-  <threadedComment ref="Q2" dT="2020-06-17T10:27:14.33" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{A6DF340C-D9B4-4213-B8D0-BC13399B784F}">
+  <threadedComment ref="T2" dT="2020-06-17T10:27:14.33" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{A6DF340C-D9B4-4213-B8D0-BC13399B784F}">
     <text>Crop (grass) - late flight period</text>
   </threadedComment>
-  <threadedComment ref="R2" dT="2020-06-17T10:27:22.63" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{C439AAA7-ACD4-4DF7-9B88-A19F61BEE251}">
+  <threadedComment ref="W2" dT="2020-06-17T10:27:22.63" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{C439AAA7-ACD4-4DF7-9B88-A19F61BEE251}">
     <text>Hedge nest</text>
   </threadedComment>
-  <threadedComment ref="S2" dT="2020-06-17T10:27:26.08" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{4DEAFCB3-D3C5-467A-B77C-9D5987F93123}">
+  <threadedComment ref="X2" dT="2020-06-17T10:27:26.08" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{4DEAFCB3-D3C5-467A-B77C-9D5987F93123}">
     <text>Hedge nest</text>
   </threadedComment>
-  <threadedComment ref="T2" dT="2020-06-17T10:27:28.66" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{751B814D-5DC3-49BB-998F-BF86DA7FC664}">
+  <threadedComment ref="Y2" dT="2020-06-17T10:27:28.66" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{751B814D-5DC3-49BB-998F-BF86DA7FC664}">
     <text>Hedge nest</text>
   </threadedComment>
-  <threadedComment ref="U2" dT="2020-06-17T10:27:38.56" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{CE003D41-2E14-4AC4-A2B7-989C38B416B0}">
+  <threadedComment ref="Z2" dT="2020-06-17T10:27:38.56" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{CE003D41-2E14-4AC4-A2B7-989C38B416B0}">
     <text>Margin nest</text>
   </threadedComment>
-  <threadedComment ref="V2" dT="2020-06-17T10:27:41.16" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{0D12942F-1149-41D9-9FCC-B574F659E0C5}">
+  <threadedComment ref="AA2" dT="2020-06-17T10:27:41.16" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{0D12942F-1149-41D9-9FCC-B574F659E0C5}">
     <text>Margin nest</text>
   </threadedComment>
-  <threadedComment ref="W2" dT="2020-06-17T10:27:43.48" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{BF4C582D-E615-4D2B-8FA2-B3377ED3A651}">
+  <threadedComment ref="AB2" dT="2020-06-17T10:27:43.48" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{BF4C582D-E615-4D2B-8FA2-B3377ED3A651}">
     <text>Margin nest</text>
   </threadedComment>
-  <threadedComment ref="X2" dT="2020-06-17T10:28:36.71" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{577817A3-41CF-4B09-B701-1DA64D94A3F7}">
+  <threadedComment ref="AC2" dT="2020-06-17T10:28:36.71" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{577817A3-41CF-4B09-B701-1DA64D94A3F7}">
     <text>Margin nest</text>
   </threadedComment>
-  <threadedComment ref="Y2" dT="2020-06-17T10:27:54.75" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{61328AAB-8080-40A5-BB72-DE3F063064D6}">
+  <threadedComment ref="AD2" dT="2020-06-17T10:27:54.75" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{61328AAB-8080-40A5-BB72-DE3F063064D6}">
     <text>Crop (arable) nest</text>
   </threadedComment>
-  <threadedComment ref="Z2" dT="2020-06-17T10:28:16.09" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{08D8BC3C-7DE2-46DE-A501-79F9B77FC5A6}">
+  <threadedComment ref="AE2" dT="2020-06-17T10:28:16.09" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{08D8BC3C-7DE2-46DE-A501-79F9B77FC5A6}">
     <text>Crop (grass) nest</text>
   </threadedComment>
-  <threadedComment ref="AA2" dT="2020-06-17T10:28:18.78" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{60F49050-15F0-4A01-B60D-D08CFC1500EA}">
+  <threadedComment ref="AF2" dT="2020-06-17T10:28:18.78" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{60F49050-15F0-4A01-B60D-D08CFC1500EA}">
     <text>Crop (grass) nest</text>
   </threadedComment>
-  <threadedComment ref="AB2" dT="2020-06-17T10:28:21.43" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{53B38088-2842-4886-AD04-FB278DF6E6D5}">
+  <threadedComment ref="AG2" dT="2020-06-17T10:28:21.43" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{53B38088-2842-4886-AD04-FB278DF6E6D5}">
     <text>Crop (grass) nest</text>
   </threadedComment>
-  <threadedComment ref="AC2" dT="2020-06-17T10:28:24.74" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{E625A537-1514-4930-ADE3-685B712C12DD}">
+  <threadedComment ref="AH2" dT="2020-06-17T10:28:24.74" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{E625A537-1514-4930-ADE3-685B712C12DD}">
     <text>Crop (grass) nest</text>
   </threadedComment>
-  <threadedComment ref="AD2" dT="2020-06-17T10:30:15.35" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{2B82472E-59FF-4148-AB12-C02672624F2E}">
+  <threadedComment ref="AK2" dT="2020-06-17T10:30:15.35" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{2B82472E-59FF-4148-AB12-C02672624F2E}">
     <text>Hedge - plants associated with damp areas specifically</text>
   </threadedComment>
-  <threadedComment ref="AE2" dT="2020-06-17T10:30:22.42" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{74099FC7-8ABC-4BCA-B048-586D8C2AB079}">
+  <threadedComment ref="AL2" dT="2020-06-17T10:30:22.42" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{74099FC7-8ABC-4BCA-B048-586D8C2AB079}">
     <text>Margin - plants associated with damp areas specifically</text>
   </threadedComment>
-  <threadedComment ref="AF2" dT="2020-06-17T10:30:30.20" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{48C3A0E7-35F7-49D1-B02F-BFD8904E48CB}">
+  <threadedComment ref="AM2" dT="2020-06-17T10:30:30.20" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{48C3A0E7-35F7-49D1-B02F-BFD8904E48CB}">
     <text>Crop (arable) - plants associated with damp areas specifically</text>
   </threadedComment>
-  <threadedComment ref="AG2" dT="2020-06-17T10:30:37.43" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{90E5597C-0F3C-4878-B496-32CD19452B20}">
+  <threadedComment ref="AN2" dT="2020-06-17T10:30:37.43" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{90E5597C-0F3C-4878-B496-32CD19452B20}">
     <text>Crop (grass) - plants associated with damp areas specifically</text>
   </threadedComment>
-  <threadedComment ref="D3" dT="2020-09-10T14:58:25.44" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{C1BDF87D-1D41-44ED-9DB5-82CE7A80DFFC}">
+  <threadedComment ref="E3" dT="2020-09-10T14:58:25.44" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{C1BDF87D-1D41-44ED-9DB5-82CE7A80DFFC}">
     <text>these cells should only have a -1 in them if the change results in a loss of forage plants in the remaining forage habitat (i.e. a reduction in forage quality). If a change results in a loss of foraging habitat but the quality of the remaining habitat is unchanged, then only the relevant cells in columns F:Q should be ascribed a -1.</text>
   </threadedComment>
   <threadedComment ref="A10" dT="2020-07-16T14:10:47.75" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{919F0F71-488C-4B09-B04F-C0CB089704D3}">
@@ -4943,10 +4949,10 @@
   <threadedComment ref="A13" dT="2020-07-10T09:01:24.04" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{2C820375-A42D-4262-80A1-2BCE47B12469}">
     <text>ww to spring linseed</text>
   </threadedComment>
-  <threadedComment ref="D13" dT="2020-07-10T09:24:06.14" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{48C6BB13-E6DC-42AB-B35A-0607696151B4}">
+  <threadedComment ref="E13" dT="2020-07-10T09:24:06.14" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{48C6BB13-E6DC-42AB-B35A-0607696151B4}">
     <text>spring linseed is a flowering crop, and less chemicals are used on it (ABC 2019)</text>
   </threadedComment>
-  <threadedComment ref="M13" dT="2020-07-10T08:57:21.19" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{7435BEBC-43A5-4387-A373-041298C99067}">
+  <threadedComment ref="P13" dT="2020-07-10T08:57:21.19" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{7435BEBC-43A5-4387-A373-041298C99067}">
     <text>spring linseed flowers in June/July
 See here:
 https://www.premiumcrops.com/files/Linseed_Guide_Final_2017_-_4.pdf</text>
@@ -4954,10 +4960,10 @@
   <threadedComment ref="A14" dT="2020-07-10T09:01:29.08" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{B90171A6-A4A6-4C45-9636-6DBA881F7A4A}">
     <text>ww to spring beans</text>
   </threadedComment>
-  <threadedComment ref="D14" dT="2020-07-10T09:26:44.27" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{6B5EBF82-CF92-4DE1-87B1-3D2CA880033A}">
+  <threadedComment ref="E14" dT="2020-07-10T09:26:44.27" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{6B5EBF82-CF92-4DE1-87B1-3D2CA880033A}">
     <text>beans are a flowering crop, plus crop protection for beans is lower (ww = £240/ha, sprbean = £125/ha, ABC 2019)</text>
   </threadedComment>
-  <threadedComment ref="L14" dT="2020-07-10T09:30:44.44" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{1C676EBF-A20E-40B0-8CCD-00E3E4D6F477}">
+  <threadedComment ref="O14" dT="2020-07-10T09:30:44.44" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{1C676EBF-A20E-40B0-8CCD-00E3E4D6F477}">
     <text>spring beans flower in May in the UK</text>
   </threadedComment>
 </ThreadedComments>
@@ -4965,38 +4971,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64F6D29A-951C-4B7B-AAD7-CC63BC8BEE38}">
-  <dimension ref="A1:AG88"/>
+  <dimension ref="A1:AO88"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
+      <selection pane="bottomLeft" activeCell="AG9" sqref="AG9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="19.33203125" style="1" customWidth="1"/>
-    <col min="2" max="18" width="3.83203125" customWidth="1"/>
-    <col min="19" max="19" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="26" width="6.6640625" customWidth="1"/>
-    <col min="27" max="27" width="8.1640625" customWidth="1"/>
-    <col min="28" max="29" width="6.6640625" customWidth="1"/>
-    <col min="30" max="33" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.1640625" style="41" customWidth="1"/>
+    <col min="3" max="6" width="3.83203125" customWidth="1"/>
+    <col min="7" max="8" width="5.6640625" style="41" customWidth="1"/>
+    <col min="9" max="20" width="3.83203125" customWidth="1"/>
+    <col min="21" max="22" width="6.6640625" style="41" customWidth="1"/>
+    <col min="23" max="23" width="3.83203125" customWidth="1"/>
+    <col min="24" max="24" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="31" width="6.6640625" customWidth="1"/>
+    <col min="32" max="32" width="8.1640625" customWidth="1"/>
+    <col min="33" max="34" width="6.6640625" customWidth="1"/>
+    <col min="35" max="36" width="6.6640625" style="41" customWidth="1"/>
+    <col min="37" max="40" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="8.83203125" style="41"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" s="27" customFormat="1" ht="32.75" customHeight="1">
+    <row r="1" spans="1:41" s="27" customFormat="1" ht="32.75" customHeight="1">
       <c r="A1" s="26"/>
-      <c r="B1" s="46" t="s">
-        <v>133</v>
-      </c>
-      <c r="C1" s="46"/>
+      <c r="C1" s="46" t="s">
+        <v>129</v>
+      </c>
       <c r="D1" s="46"/>
       <c r="E1" s="46"/>
-      <c r="F1" s="46" t="s">
-        <v>70</v>
-      </c>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="I1" s="46" t="s">
+        <v>66</v>
+      </c>
       <c r="J1" s="46"/>
       <c r="K1" s="46"/>
       <c r="L1" s="46"/>
@@ -5005,164 +5015,189 @@
       <c r="O1" s="46"/>
       <c r="P1" s="46"/>
       <c r="Q1" s="46"/>
-      <c r="R1" s="46" t="s">
-        <v>138</v>
-      </c>
+      <c r="R1" s="46"/>
       <c r="S1" s="46"/>
       <c r="T1" s="46"/>
-      <c r="U1" s="46"/>
-      <c r="V1" s="46"/>
-      <c r="W1" s="46"/>
+      <c r="V1" s="44"/>
+      <c r="W1" s="46" t="s">
+        <v>134</v>
+      </c>
       <c r="X1" s="46"/>
       <c r="Y1" s="46"/>
       <c r="Z1" s="46"/>
       <c r="AA1" s="46"/>
       <c r="AB1" s="46"/>
       <c r="AC1" s="46"/>
-      <c r="AD1" s="47" t="s">
-        <v>139</v>
-      </c>
-      <c r="AE1" s="47"/>
-      <c r="AF1" s="47"/>
-      <c r="AG1" s="47"/>
-    </row>
-    <row r="2" spans="1:33" s="4" customFormat="1" ht="114.5" customHeight="1">
+      <c r="AD1" s="46"/>
+      <c r="AE1" s="46"/>
+      <c r="AF1" s="46"/>
+      <c r="AG1" s="46"/>
+      <c r="AH1" s="46"/>
+      <c r="AI1" s="51"/>
+      <c r="AJ1" s="51"/>
+      <c r="AK1" s="47" t="s">
+        <v>135</v>
+      </c>
+      <c r="AL1" s="47"/>
+      <c r="AM1" s="47"/>
+      <c r="AN1" s="47"/>
+      <c r="AO1" s="53"/>
+    </row>
+    <row r="2" spans="1:41" s="4" customFormat="1" ht="114.5" customHeight="1">
       <c r="A2" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="41" t="s">
+        <v>190</v>
+      </c>
+      <c r="C2" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="15" t="s">
-        <v>35</v>
-      </c>
       <c r="D2" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="E2" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="F2" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" s="43" t="s">
+        <v>191</v>
+      </c>
+      <c r="H2" s="43" t="s">
+        <v>192</v>
+      </c>
+      <c r="I2" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="J2" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="K2" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="L2" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="J2" s="13" t="s">
+      <c r="M2" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="K2" s="13" t="s">
+      <c r="N2" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="L2" s="13" t="s">
+      <c r="O2" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="M2" s="13" t="s">
+      <c r="P2" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="N2" s="13" t="s">
+      <c r="Q2" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="O2" s="13" t="s">
+      <c r="R2" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="P2" s="13" t="s">
+      <c r="S2" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="Q2" s="13" t="s">
+      <c r="T2" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="R2" s="12" t="s">
+      <c r="U2" s="44" t="s">
+        <v>193</v>
+      </c>
+      <c r="V2" s="41" t="s">
+        <v>196</v>
+      </c>
+      <c r="W2" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="S2" s="12" t="s">
+      <c r="X2" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="T2" s="11" t="s">
+      <c r="Y2" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="U2" s="10" t="s">
+      <c r="Z2" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="V2" s="10" t="s">
+      <c r="AA2" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="W2" s="10" t="s">
+      <c r="AB2" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="X2" s="9" t="s">
+      <c r="AC2" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="Y2" s="8" t="s">
+      <c r="AD2" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="Z2" s="7" t="s">
+      <c r="AE2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="AA2" s="7" t="s">
+      <c r="AF2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="AB2" s="7" t="s">
+      <c r="AG2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="AC2" s="6" t="s">
+      <c r="AH2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="AD2" s="5" t="s">
+      <c r="AI2" s="52" t="s">
+        <v>197</v>
+      </c>
+      <c r="AJ2" s="52" t="s">
+        <v>194</v>
+      </c>
+      <c r="AK2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="AE2" s="5" t="s">
+      <c r="AL2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="AF2" s="5" t="s">
+      <c r="AM2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="AG2" s="5" t="s">
+      <c r="AN2" s="5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:33" ht="16">
+      <c r="AO2" s="54" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="3" spans="1:41" ht="16">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="25">
-        <v>-1</v>
-      </c>
-      <c r="E3" s="3"/>
-      <c r="N3">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:33" ht="16">
+      <c r="B3" s="42"/>
+      <c r="E3" s="25">
+        <v>-1</v>
+      </c>
+      <c r="F3" s="3"/>
+      <c r="Q3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:41" ht="16">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="25">
-        <v>-1</v>
-      </c>
+      <c r="B4" s="42"/>
       <c r="E4" s="25">
         <v>-1</v>
       </c>
-    </row>
-    <row r="5" spans="1:33" ht="16">
+      <c r="F4" s="25">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:41" ht="16">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F5">
-        <v>-1</v>
-      </c>
-      <c r="G5">
-        <v>-1</v>
-      </c>
-      <c r="H5">
-        <v>-1</v>
-      </c>
+      <c r="B5" s="42"/>
       <c r="I5">
         <v>-1</v>
       </c>
@@ -5172,848 +5207,870 @@
       <c r="K5">
         <v>-1</v>
       </c>
-      <c r="V5">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:33" ht="16">
+      <c r="L5">
+        <v>-1</v>
+      </c>
+      <c r="M5">
+        <v>-1</v>
+      </c>
+      <c r="N5">
+        <v>-1</v>
+      </c>
+      <c r="AA5">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:41" ht="16">
       <c r="A6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="I6">
-        <v>-1</v>
-      </c>
-      <c r="J6">
-        <v>-1</v>
-      </c>
-      <c r="K6">
-        <v>-1</v>
-      </c>
-      <c r="AD6">
-        <v>-1</v>
-      </c>
-      <c r="AE6">
-        <v>-1</v>
-      </c>
-      <c r="AF6">
-        <v>-1</v>
-      </c>
-      <c r="AG6">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:33" ht="16">
+      <c r="B6" s="42"/>
+      <c r="L6">
+        <v>-1</v>
+      </c>
+      <c r="M6">
+        <v>-1</v>
+      </c>
+      <c r="N6">
+        <v>-1</v>
+      </c>
+      <c r="AK6">
+        <v>-1</v>
+      </c>
+      <c r="AL6">
+        <v>-1</v>
+      </c>
+      <c r="AM6">
+        <v>-1</v>
+      </c>
+      <c r="AN6">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:41" ht="16">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="N7">
-        <v>-1</v>
-      </c>
-      <c r="O7">
-        <v>-1</v>
-      </c>
-      <c r="P7">
-        <v>-1</v>
-      </c>
+      <c r="B7" s="42"/>
       <c r="Q7">
         <v>-1</v>
       </c>
-      <c r="AA7">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:33">
-      <c r="A8" s="2"/>
-    </row>
-    <row r="9" spans="1:33">
+      <c r="R7">
+        <v>-1</v>
+      </c>
+      <c r="S7">
+        <v>-1</v>
+      </c>
+      <c r="T7">
+        <v>-1</v>
+      </c>
+      <c r="AF7">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:41" ht="16">
+      <c r="A8" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="F8">
+        <v>-1</v>
+      </c>
+      <c r="AF8">
+        <v>-1</v>
+      </c>
+      <c r="AG8">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:41">
       <c r="A9" s="2"/>
     </row>
-    <row r="10" spans="1:33">
+    <row r="10" spans="1:41">
       <c r="A10" s="24"/>
-      <c r="B10" s="23"/>
-    </row>
-    <row r="11" spans="1:33">
+      <c r="C10" s="23"/>
+    </row>
+    <row r="11" spans="1:41">
       <c r="A11" s="24"/>
-      <c r="B11" s="22"/>
-    </row>
-    <row r="12" spans="1:33">
+      <c r="C11" s="22"/>
+    </row>
+    <row r="12" spans="1:41">
       <c r="A12" s="2"/>
     </row>
-    <row r="13" spans="1:33" ht="16">
+    <row r="13" spans="1:41" ht="16">
       <c r="A13" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="D13">
+        <v>124</v>
+      </c>
+      <c r="E13">
         <v>1</v>
       </c>
-      <c r="M13">
+      <c r="P13">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:33" ht="16">
+    <row r="14" spans="1:41" ht="16">
       <c r="A14" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="D14">
+        <v>125</v>
+      </c>
+      <c r="E14">
         <v>1</v>
       </c>
-      <c r="L14">
+      <c r="O14">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:33">
+    <row r="15" spans="1:41">
       <c r="A15" s="2"/>
     </row>
-    <row r="16" spans="1:33">
+    <row r="16" spans="1:41">
       <c r="A16" s="2"/>
     </row>
-    <row r="17" spans="1:17" ht="16">
+    <row r="17" spans="1:20" ht="16">
       <c r="A17" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="E17" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F17" s="3"/>
+      <c r="Q17">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" ht="16">
+      <c r="A18" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="E18" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F18" s="3">
+        <v>-1</v>
+      </c>
+      <c r="O18">
+        <v>-1</v>
+      </c>
+      <c r="P18">
+        <v>-1</v>
+      </c>
+      <c r="Q18">
+        <v>-1</v>
+      </c>
+      <c r="R18">
+        <v>-1</v>
+      </c>
+      <c r="S18">
+        <v>-1</v>
+      </c>
+      <c r="T18">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" ht="16">
+      <c r="A19" s="28" t="s">
+        <v>138</v>
+      </c>
+      <c r="E19" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F19" s="3"/>
+      <c r="Q19">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" ht="16">
+      <c r="A20" s="28" t="s">
+        <v>139</v>
+      </c>
+      <c r="E20" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F20" s="3">
+        <v>-1</v>
+      </c>
+      <c r="O20">
+        <v>-1</v>
+      </c>
+      <c r="P20">
+        <v>-1</v>
+      </c>
+      <c r="Q20">
+        <v>-1</v>
+      </c>
+      <c r="R20">
+        <v>-1</v>
+      </c>
+      <c r="S20">
+        <v>-1</v>
+      </c>
+      <c r="T20">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" ht="16">
+      <c r="A21" s="28" t="s">
         <v>140</v>
       </c>
-      <c r="D17" s="3">
-        <v>-1</v>
-      </c>
-      <c r="E17" s="3"/>
-      <c r="N17">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" ht="16">
-      <c r="A18" s="28" t="s">
+      <c r="E21" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F21" s="3"/>
+      <c r="Q21">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" ht="16">
+      <c r="A22" s="28" t="s">
         <v>141</v>
       </c>
-      <c r="D18" s="3">
-        <v>-1</v>
-      </c>
-      <c r="E18" s="3">
-        <v>-1</v>
-      </c>
-      <c r="L18">
-        <v>-1</v>
-      </c>
-      <c r="M18">
-        <v>-1</v>
-      </c>
-      <c r="N18">
-        <v>-1</v>
-      </c>
-      <c r="O18">
-        <v>-1</v>
-      </c>
-      <c r="P18">
-        <v>-1</v>
-      </c>
-      <c r="Q18">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" ht="16">
-      <c r="A19" s="28" t="s">
+      <c r="E22" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F22" s="3">
+        <v>-1</v>
+      </c>
+      <c r="O22">
+        <v>-1</v>
+      </c>
+      <c r="P22">
+        <v>-1</v>
+      </c>
+      <c r="Q22">
+        <v>-1</v>
+      </c>
+      <c r="R22">
+        <v>-1</v>
+      </c>
+      <c r="S22">
+        <v>-1</v>
+      </c>
+      <c r="T22">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" ht="16">
+      <c r="A23" s="28" t="s">
         <v>142</v>
       </c>
-      <c r="D19" s="3">
-        <v>-1</v>
-      </c>
-      <c r="E19" s="3"/>
-      <c r="N19">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" ht="16">
-      <c r="A20" s="28" t="s">
+      <c r="E23" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F23" s="3"/>
+      <c r="Q23">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" ht="16">
+      <c r="A24" s="28" t="s">
         <v>143</v>
       </c>
-      <c r="D20" s="3">
-        <v>-1</v>
-      </c>
-      <c r="E20" s="3">
-        <v>-1</v>
-      </c>
-      <c r="L20">
-        <v>-1</v>
-      </c>
-      <c r="M20">
-        <v>-1</v>
-      </c>
-      <c r="N20">
-        <v>-1</v>
-      </c>
-      <c r="O20">
-        <v>-1</v>
-      </c>
-      <c r="P20">
-        <v>-1</v>
-      </c>
-      <c r="Q20">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" ht="16">
-      <c r="A21" s="28" t="s">
+      <c r="E24" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F24" s="3">
+        <v>-1</v>
+      </c>
+      <c r="O24">
+        <v>-1</v>
+      </c>
+      <c r="P24">
+        <v>-1</v>
+      </c>
+      <c r="Q24">
+        <v>-1</v>
+      </c>
+      <c r="R24">
+        <v>-1</v>
+      </c>
+      <c r="S24">
+        <v>-1</v>
+      </c>
+      <c r="T24">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" ht="16">
+      <c r="A25" s="28" t="s">
         <v>144</v>
       </c>
-      <c r="D21" s="3">
-        <v>-1</v>
-      </c>
-      <c r="E21" s="3"/>
-      <c r="N21">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" ht="16">
-      <c r="A22" s="28" t="s">
+      <c r="E25" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F25" s="3"/>
+      <c r="Q25">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" ht="16">
+      <c r="A26" s="28" t="s">
         <v>145</v>
       </c>
-      <c r="D22" s="3">
-        <v>-1</v>
-      </c>
-      <c r="E22" s="3">
-        <v>-1</v>
-      </c>
-      <c r="L22">
-        <v>-1</v>
-      </c>
-      <c r="M22">
-        <v>-1</v>
-      </c>
-      <c r="N22">
-        <v>-1</v>
-      </c>
-      <c r="O22">
-        <v>-1</v>
-      </c>
-      <c r="P22">
-        <v>-1</v>
-      </c>
-      <c r="Q22">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" ht="16">
-      <c r="A23" s="28" t="s">
+      <c r="E26" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F26" s="3">
+        <v>-1</v>
+      </c>
+      <c r="O26">
+        <v>-1</v>
+      </c>
+      <c r="P26">
+        <v>-1</v>
+      </c>
+      <c r="Q26">
+        <v>-1</v>
+      </c>
+      <c r="R26">
+        <v>-1</v>
+      </c>
+      <c r="S26">
+        <v>-1</v>
+      </c>
+      <c r="T26">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" ht="16">
+      <c r="A27" s="28" t="s">
         <v>146</v>
       </c>
-      <c r="D23" s="3">
-        <v>-1</v>
-      </c>
-      <c r="E23" s="3"/>
-      <c r="N23">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" ht="16">
-      <c r="A24" s="28" t="s">
+      <c r="E27" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F27" s="3"/>
+      <c r="Q27">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" ht="16">
+      <c r="A28" s="28" t="s">
         <v>147</v>
       </c>
-      <c r="D24" s="3">
-        <v>-1</v>
-      </c>
-      <c r="E24" s="3">
-        <v>-1</v>
-      </c>
-      <c r="L24">
-        <v>-1</v>
-      </c>
-      <c r="M24">
-        <v>-1</v>
-      </c>
-      <c r="N24">
-        <v>-1</v>
-      </c>
-      <c r="O24">
-        <v>-1</v>
-      </c>
-      <c r="P24">
-        <v>-1</v>
-      </c>
-      <c r="Q24">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" ht="16">
-      <c r="A25" s="28" t="s">
+      <c r="E28" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F28" s="3">
+        <v>-1</v>
+      </c>
+      <c r="O28">
+        <v>-1</v>
+      </c>
+      <c r="P28">
+        <v>-1</v>
+      </c>
+      <c r="Q28">
+        <v>-1</v>
+      </c>
+      <c r="R28">
+        <v>-1</v>
+      </c>
+      <c r="S28">
+        <v>-1</v>
+      </c>
+      <c r="T28">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20">
+      <c r="A29" s="28"/>
+    </row>
+    <row r="30" spans="1:20">
+      <c r="A30" s="28"/>
+    </row>
+    <row r="31" spans="1:20" ht="32">
+      <c r="A31" s="29" t="s">
         <v>148</v>
       </c>
-      <c r="D25" s="3">
-        <v>-1</v>
-      </c>
-      <c r="E25" s="3"/>
-      <c r="N25">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" ht="16">
-      <c r="A26" s="28" t="s">
+    </row>
+    <row r="32" spans="1:20" ht="16">
+      <c r="A32" s="30" t="s">
         <v>149</v>
       </c>
-      <c r="D26" s="3">
-        <v>-1</v>
-      </c>
-      <c r="E26" s="3">
-        <v>-1</v>
-      </c>
-      <c r="L26">
-        <v>-1</v>
-      </c>
-      <c r="M26">
-        <v>-1</v>
-      </c>
-      <c r="N26">
-        <v>-1</v>
-      </c>
-      <c r="O26">
-        <v>-1</v>
-      </c>
-      <c r="P26">
-        <v>-1</v>
-      </c>
-      <c r="Q26">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" ht="16">
-      <c r="A27" s="28" t="s">
+      <c r="E32" s="31"/>
+      <c r="P32" s="31"/>
+    </row>
+    <row r="33" spans="1:20" ht="16">
+      <c r="A33" s="30" t="s">
         <v>150</v>
       </c>
-      <c r="D27" s="3">
-        <v>-1</v>
-      </c>
-      <c r="E27" s="3"/>
-      <c r="N27">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" ht="16">
-      <c r="A28" s="28" t="s">
+      <c r="E33" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F33" s="3">
+        <v>-1</v>
+      </c>
+      <c r="O33">
+        <v>-1</v>
+      </c>
+      <c r="P33">
+        <v>-1</v>
+      </c>
+      <c r="Q33">
+        <v>-1</v>
+      </c>
+      <c r="R33">
+        <v>-1</v>
+      </c>
+      <c r="S33">
+        <v>-1</v>
+      </c>
+      <c r="T33">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" ht="32">
+      <c r="A34" s="30" t="s">
         <v>151</v>
       </c>
-      <c r="D28" s="3">
-        <v>-1</v>
-      </c>
-      <c r="E28" s="3">
-        <v>-1</v>
-      </c>
-      <c r="L28">
-        <v>-1</v>
-      </c>
-      <c r="M28">
-        <v>-1</v>
-      </c>
-      <c r="N28">
-        <v>-1</v>
-      </c>
-      <c r="O28">
-        <v>-1</v>
-      </c>
-      <c r="P28">
-        <v>-1</v>
-      </c>
-      <c r="Q28">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17">
-      <c r="A29" s="28"/>
-    </row>
-    <row r="30" spans="1:17">
-      <c r="A30" s="28"/>
-    </row>
-    <row r="31" spans="1:17" ht="32">
-      <c r="A31" s="29" t="s">
+      <c r="E34" s="31"/>
+      <c r="O34" s="31"/>
+    </row>
+    <row r="35" spans="1:20" ht="32">
+      <c r="A35" s="30" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="32" spans="1:17" ht="16">
-      <c r="A32" s="30" t="s">
+      <c r="E35" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F35" s="3">
+        <v>-1</v>
+      </c>
+      <c r="O35">
+        <v>-1</v>
+      </c>
+      <c r="P35">
+        <v>-1</v>
+      </c>
+      <c r="Q35">
+        <v>-1</v>
+      </c>
+      <c r="R35">
+        <v>-1</v>
+      </c>
+      <c r="S35">
+        <v>-1</v>
+      </c>
+      <c r="T35">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" ht="16">
+      <c r="A36" s="30" t="s">
         <v>153</v>
       </c>
-      <c r="D32" s="31"/>
-      <c r="M32" s="31"/>
-    </row>
-    <row r="33" spans="1:17" ht="16">
-      <c r="A33" s="30" t="s">
+      <c r="E36">
+        <v>-1</v>
+      </c>
+      <c r="O36">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" ht="16">
+      <c r="A37" s="30" t="s">
         <v>154</v>
       </c>
-      <c r="D33" s="3">
-        <v>-1</v>
-      </c>
-      <c r="E33" s="3">
-        <v>-1</v>
-      </c>
-      <c r="L33">
-        <v>-1</v>
-      </c>
-      <c r="M33">
-        <v>-1</v>
-      </c>
-      <c r="N33">
-        <v>-1</v>
-      </c>
-      <c r="O33">
-        <v>-1</v>
-      </c>
-      <c r="P33">
-        <v>-1</v>
-      </c>
-      <c r="Q33">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:17" ht="32">
-      <c r="A34" s="30" t="s">
+      <c r="E37" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F37" s="3">
+        <v>-1</v>
+      </c>
+      <c r="O37">
+        <v>-1</v>
+      </c>
+      <c r="P37">
+        <v>-1</v>
+      </c>
+      <c r="Q37">
+        <v>-1</v>
+      </c>
+      <c r="R37">
+        <v>-1</v>
+      </c>
+      <c r="S37">
+        <v>-1</v>
+      </c>
+      <c r="T37">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" ht="16">
+      <c r="A38" s="30" t="s">
         <v>155</v>
       </c>
-      <c r="D34" s="31"/>
-      <c r="L34" s="31"/>
-    </row>
-    <row r="35" spans="1:17" ht="32">
-      <c r="A35" s="30" t="s">
+      <c r="E38" s="31"/>
+    </row>
+    <row r="39" spans="1:20">
+      <c r="A39" s="30"/>
+      <c r="E39" s="31"/>
+    </row>
+    <row r="40" spans="1:20" ht="16">
+      <c r="A40" s="30" t="s">
         <v>156</v>
       </c>
-      <c r="D35" s="3">
-        <v>-1</v>
-      </c>
-      <c r="E35" s="3">
-        <v>-1</v>
-      </c>
-      <c r="L35">
-        <v>-1</v>
-      </c>
-      <c r="M35">
-        <v>-1</v>
-      </c>
-      <c r="N35">
-        <v>-1</v>
-      </c>
-      <c r="O35">
-        <v>-1</v>
-      </c>
-      <c r="P35">
-        <v>-1</v>
-      </c>
-      <c r="Q35">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:17" ht="16">
-      <c r="A36" s="30" t="s">
+    </row>
+    <row r="41" spans="1:20" ht="16">
+      <c r="A41" s="30" t="s">
         <v>157</v>
       </c>
-      <c r="D36">
-        <v>-1</v>
-      </c>
-      <c r="L36">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:17" ht="16">
-      <c r="A37" s="30" t="s">
+      <c r="E41" s="31"/>
+      <c r="O41">
+        <v>-1</v>
+      </c>
+      <c r="P41" s="31"/>
+    </row>
+    <row r="42" spans="1:20" ht="16">
+      <c r="A42" s="32" t="s">
         <v>158</v>
       </c>
-      <c r="D37" s="3">
-        <v>-1</v>
-      </c>
-      <c r="E37" s="3">
-        <v>-1</v>
-      </c>
-      <c r="L37">
-        <v>-1</v>
-      </c>
-      <c r="M37">
-        <v>-1</v>
-      </c>
-      <c r="N37">
-        <v>-1</v>
-      </c>
-      <c r="O37">
-        <v>-1</v>
-      </c>
-      <c r="P37">
-        <v>-1</v>
-      </c>
-      <c r="Q37">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:17" ht="16">
-      <c r="A38" s="30" t="s">
+      <c r="E42" s="31"/>
+      <c r="P42" s="31"/>
+    </row>
+    <row r="43" spans="1:20" ht="16">
+      <c r="A43" s="30" t="s">
         <v>159</v>
       </c>
-      <c r="D38" s="31"/>
-    </row>
-    <row r="39" spans="1:17">
-      <c r="A39" s="30"/>
-      <c r="D39" s="31"/>
-    </row>
-    <row r="40" spans="1:17" ht="16">
-      <c r="A40" s="30" t="s">
+      <c r="E43" s="31"/>
+      <c r="O43" s="31"/>
+      <c r="P43" s="31"/>
+    </row>
+    <row r="44" spans="1:20" ht="16">
+      <c r="A44" s="30" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="41" spans="1:17" ht="16">
-      <c r="A41" s="30" t="s">
+      <c r="E44" s="33">
+        <v>-1</v>
+      </c>
+      <c r="O44">
+        <v>-1</v>
+      </c>
+      <c r="P44" s="31"/>
+    </row>
+    <row r="45" spans="1:20" ht="16">
+      <c r="A45" s="30" t="s">
         <v>161</v>
       </c>
-      <c r="D41" s="31"/>
-      <c r="L41">
-        <v>-1</v>
-      </c>
-      <c r="M41" s="31"/>
-    </row>
-    <row r="42" spans="1:17" ht="16">
-      <c r="A42" s="32" t="s">
+      <c r="E45" s="31"/>
+      <c r="P45" s="31"/>
+    </row>
+    <row r="46" spans="1:20" ht="14.75" customHeight="1">
+      <c r="A46" s="30" t="s">
         <v>162</v>
       </c>
-      <c r="D42" s="31"/>
-      <c r="M42" s="31"/>
-    </row>
-    <row r="43" spans="1:17" ht="16">
-      <c r="A43" s="30" t="s">
+      <c r="E46" s="31"/>
+      <c r="O46" s="31"/>
+      <c r="P46" s="31"/>
+    </row>
+    <row r="47" spans="1:20" ht="16">
+      <c r="A47" s="30" t="s">
         <v>163</v>
       </c>
-      <c r="D43" s="31"/>
-      <c r="L43" s="31"/>
-      <c r="M43" s="31"/>
-    </row>
-    <row r="44" spans="1:17" ht="16">
-      <c r="A44" s="30" t="s">
+      <c r="E47" s="33">
+        <v>-1</v>
+      </c>
+      <c r="O47">
+        <v>-1</v>
+      </c>
+      <c r="P47" s="31"/>
+    </row>
+    <row r="48" spans="1:20" ht="16">
+      <c r="A48" s="28" t="s">
         <v>164</v>
       </c>
-      <c r="D44" s="33">
-        <v>-1</v>
-      </c>
-      <c r="L44">
-        <v>-1</v>
-      </c>
-      <c r="M44" s="31"/>
-    </row>
-    <row r="45" spans="1:17" ht="16">
-      <c r="A45" s="30" t="s">
+    </row>
+    <row r="49" spans="1:15" ht="16">
+      <c r="A49" s="28" t="s">
         <v>165</v>
       </c>
-      <c r="D45" s="31"/>
-      <c r="M45" s="31"/>
-    </row>
-    <row r="46" spans="1:17" ht="14.75" customHeight="1">
-      <c r="A46" s="30" t="s">
+      <c r="E49" s="31"/>
+      <c r="O49" s="31"/>
+    </row>
+    <row r="50" spans="1:15" ht="16">
+      <c r="A50" s="28" t="s">
         <v>166</v>
       </c>
-      <c r="D46" s="31"/>
-      <c r="L46" s="31"/>
-      <c r="M46" s="31"/>
-    </row>
-    <row r="47" spans="1:17" ht="16">
-      <c r="A47" s="30" t="s">
+      <c r="E50">
+        <v>-1</v>
+      </c>
+      <c r="O50">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" ht="16">
+      <c r="A51" s="28" t="s">
         <v>167</v>
       </c>
-      <c r="D47" s="33">
-        <v>-1</v>
-      </c>
-      <c r="L47">
-        <v>-1</v>
-      </c>
-      <c r="M47" s="31"/>
-    </row>
-    <row r="48" spans="1:17" ht="16">
-      <c r="A48" s="28" t="s">
+    </row>
+    <row r="52" spans="1:15" ht="16">
+      <c r="A52" s="28" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="49" spans="1:12" ht="16">
-      <c r="A49" s="28" t="s">
+      <c r="E52" s="31"/>
+      <c r="O52" s="31"/>
+    </row>
+    <row r="53" spans="1:15" ht="16">
+      <c r="A53" s="28" t="s">
         <v>169</v>
       </c>
-      <c r="D49" s="31"/>
-      <c r="L49" s="31"/>
-    </row>
-    <row r="50" spans="1:12" ht="16">
-      <c r="A50" s="28" t="s">
+      <c r="E53">
+        <v>-1</v>
+      </c>
+      <c r="O53">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" ht="16">
+      <c r="A54" s="28" t="s">
         <v>170</v>
       </c>
-      <c r="D50">
-        <v>-1</v>
-      </c>
-      <c r="L50">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" ht="16">
-      <c r="A51" s="28" t="s">
+    </row>
+    <row r="55" spans="1:15" ht="16">
+      <c r="A55" s="28" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="52" spans="1:12" ht="16">
-      <c r="A52" s="28" t="s">
+    <row r="56" spans="1:15" ht="16">
+      <c r="A56" s="28" t="s">
         <v>172</v>
       </c>
-      <c r="D52" s="31"/>
-      <c r="L52" s="31"/>
-    </row>
-    <row r="53" spans="1:12" ht="16">
-      <c r="A53" s="28" t="s">
+      <c r="E56">
+        <v>-1</v>
+      </c>
+      <c r="O56">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" ht="16">
+      <c r="A57" s="28" t="s">
         <v>173</v>
       </c>
-      <c r="D53">
-        <v>-1</v>
-      </c>
-      <c r="L53">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12" ht="16">
-      <c r="A54" s="28" t="s">
+    </row>
+    <row r="58" spans="1:15" ht="16">
+      <c r="A58" s="28" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="55" spans="1:12" ht="16">
-      <c r="A55" s="28" t="s">
+    <row r="59" spans="1:15" ht="16">
+      <c r="A59" s="28" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="56" spans="1:12" ht="16">
-      <c r="A56" s="28" t="s">
+      <c r="E59">
+        <v>-1</v>
+      </c>
+      <c r="O59">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15">
+      <c r="A60" s="28"/>
+    </row>
+    <row r="61" spans="1:15">
+      <c r="A61" s="28"/>
+    </row>
+    <row r="62" spans="1:15">
+      <c r="A62" s="28"/>
+    </row>
+    <row r="63" spans="1:15">
+      <c r="A63" s="28"/>
+    </row>
+    <row r="64" spans="1:15" ht="32">
+      <c r="A64" s="29" t="s">
         <v>176</v>
       </c>
-      <c r="D56">
-        <v>-1</v>
-      </c>
-      <c r="L56">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12" ht="16">
-      <c r="A57" s="28" t="s">
+    </row>
+    <row r="65" spans="1:16" ht="16">
+      <c r="A65" s="30" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="58" spans="1:12" ht="16">
-      <c r="A58" s="28" t="s">
+      <c r="E65" s="31"/>
+      <c r="P65" s="31"/>
+    </row>
+    <row r="66" spans="1:16" ht="16">
+      <c r="A66" s="30" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="59" spans="1:12" ht="16">
-      <c r="A59" s="28" t="s">
+      <c r="E66" s="31"/>
+      <c r="O66" s="31"/>
+    </row>
+    <row r="67" spans="1:16" ht="16">
+      <c r="A67" s="30" t="s">
         <v>179</v>
       </c>
-      <c r="D59">
-        <v>-1</v>
-      </c>
-      <c r="L59">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12">
-      <c r="A60" s="28"/>
-    </row>
-    <row r="61" spans="1:12">
-      <c r="A61" s="28"/>
-    </row>
-    <row r="62" spans="1:12">
-      <c r="A62" s="28"/>
-    </row>
-    <row r="63" spans="1:12">
-      <c r="A63" s="28"/>
-    </row>
-    <row r="64" spans="1:12" ht="32">
-      <c r="A64" s="29" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="65" spans="1:13" ht="16">
-      <c r="A65" s="30" t="s">
-        <v>181</v>
-      </c>
-      <c r="D65" s="31"/>
-      <c r="M65" s="31"/>
-    </row>
-    <row r="66" spans="1:13" ht="16">
-      <c r="A66" s="30" t="s">
-        <v>182</v>
-      </c>
-      <c r="D66" s="31"/>
-      <c r="L66" s="31"/>
-    </row>
-    <row r="67" spans="1:13" ht="16">
-      <c r="A67" s="30" t="s">
-        <v>183</v>
-      </c>
-      <c r="D67">
-        <v>-1</v>
-      </c>
-      <c r="L67">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:13" ht="16">
+      <c r="E67">
+        <v>-1</v>
+      </c>
+      <c r="O67">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:16" ht="16">
       <c r="A68" s="30" t="s">
+        <v>155</v>
+      </c>
+      <c r="E68" s="31"/>
+    </row>
+    <row r="69" spans="1:16" ht="16">
+      <c r="A69" s="30" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="70" spans="1:16" ht="16">
+      <c r="A70" s="30" t="s">
+        <v>157</v>
+      </c>
+      <c r="E70" s="31"/>
+      <c r="O70">
+        <v>-1</v>
+      </c>
+      <c r="P70" s="31"/>
+    </row>
+    <row r="71" spans="1:16" ht="16">
+      <c r="A71" s="32" t="s">
+        <v>158</v>
+      </c>
+      <c r="E71" s="31"/>
+      <c r="P71" s="31"/>
+    </row>
+    <row r="72" spans="1:16" ht="16">
+      <c r="A72" s="30" t="s">
         <v>159</v>
       </c>
-      <c r="D68" s="31"/>
-    </row>
-    <row r="69" spans="1:13" ht="16">
-      <c r="A69" s="30" t="s">
+      <c r="E72" s="31"/>
+      <c r="O72" s="31"/>
+      <c r="P72" s="31"/>
+    </row>
+    <row r="73" spans="1:16" ht="16">
+      <c r="A73" s="30" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="70" spans="1:13" ht="16">
-      <c r="A70" s="30" t="s">
+      <c r="E73" s="33">
+        <v>-1</v>
+      </c>
+      <c r="O73">
+        <v>-1</v>
+      </c>
+      <c r="P73" s="31"/>
+    </row>
+    <row r="74" spans="1:16" ht="16">
+      <c r="A74" s="30" t="s">
         <v>161</v>
       </c>
-      <c r="D70" s="31"/>
-      <c r="L70">
-        <v>-1</v>
-      </c>
-      <c r="M70" s="31"/>
-    </row>
-    <row r="71" spans="1:13" ht="16">
-      <c r="A71" s="32" t="s">
+      <c r="E74" s="31"/>
+      <c r="P74" s="31"/>
+    </row>
+    <row r="75" spans="1:16" ht="14.75" customHeight="1">
+      <c r="A75" s="30" t="s">
         <v>162</v>
       </c>
-      <c r="D71" s="31"/>
-      <c r="M71" s="31"/>
-    </row>
-    <row r="72" spans="1:13" ht="16">
-      <c r="A72" s="30" t="s">
+      <c r="E75" s="31"/>
+      <c r="O75" s="31"/>
+      <c r="P75" s="31"/>
+    </row>
+    <row r="76" spans="1:16" ht="16">
+      <c r="A76" s="30" t="s">
         <v>163</v>
       </c>
-      <c r="D72" s="31"/>
-      <c r="L72" s="31"/>
-      <c r="M72" s="31"/>
-    </row>
-    <row r="73" spans="1:13" ht="16">
-      <c r="A73" s="30" t="s">
+      <c r="E76" s="33">
+        <v>-1</v>
+      </c>
+      <c r="O76">
+        <v>-1</v>
+      </c>
+      <c r="P76" s="31"/>
+    </row>
+    <row r="77" spans="1:16" ht="16">
+      <c r="A77" s="28" t="s">
         <v>164</v>
       </c>
-      <c r="D73" s="33">
-        <v>-1</v>
-      </c>
-      <c r="L73">
-        <v>-1</v>
-      </c>
-      <c r="M73" s="31"/>
-    </row>
-    <row r="74" spans="1:13" ht="16">
-      <c r="A74" s="30" t="s">
+    </row>
+    <row r="78" spans="1:16" ht="16">
+      <c r="A78" s="28" t="s">
         <v>165</v>
       </c>
-      <c r="D74" s="31"/>
-      <c r="M74" s="31"/>
-    </row>
-    <row r="75" spans="1:13" ht="14.75" customHeight="1">
-      <c r="A75" s="30" t="s">
+      <c r="E78" s="31"/>
+      <c r="O78" s="31"/>
+    </row>
+    <row r="79" spans="1:16" ht="16">
+      <c r="A79" s="28" t="s">
         <v>166</v>
       </c>
-      <c r="D75" s="31"/>
-      <c r="L75" s="31"/>
-      <c r="M75" s="31"/>
-    </row>
-    <row r="76" spans="1:13" ht="16">
-      <c r="A76" s="30" t="s">
+      <c r="E79">
+        <v>-1</v>
+      </c>
+      <c r="O79">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:16" ht="16">
+      <c r="A80" s="28" t="s">
         <v>167</v>
       </c>
-      <c r="D76" s="33">
-        <v>-1</v>
-      </c>
-      <c r="L76">
-        <v>-1</v>
-      </c>
-      <c r="M76" s="31"/>
-    </row>
-    <row r="77" spans="1:13" ht="16">
-      <c r="A77" s="28" t="s">
+    </row>
+    <row r="81" spans="1:15" ht="16">
+      <c r="A81" s="28" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="78" spans="1:13" ht="16">
-      <c r="A78" s="28" t="s">
+      <c r="E81" s="31"/>
+      <c r="O81" s="31"/>
+    </row>
+    <row r="82" spans="1:15" ht="16">
+      <c r="A82" s="28" t="s">
         <v>169</v>
       </c>
-      <c r="D78" s="31"/>
-      <c r="L78" s="31"/>
-    </row>
-    <row r="79" spans="1:13" ht="16">
-      <c r="A79" s="28" t="s">
+      <c r="E82">
+        <v>-1</v>
+      </c>
+      <c r="O82">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:15" ht="16">
+      <c r="A83" s="28" t="s">
         <v>170</v>
       </c>
-      <c r="D79">
-        <v>-1</v>
-      </c>
-      <c r="L79">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="80" spans="1:13" ht="16">
-      <c r="A80" s="28" t="s">
+    </row>
+    <row r="84" spans="1:15" ht="16">
+      <c r="A84" s="28" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="81" spans="1:12" ht="16">
-      <c r="A81" s="28" t="s">
+    <row r="85" spans="1:15" ht="16">
+      <c r="A85" s="28" t="s">
         <v>172</v>
       </c>
-      <c r="D81" s="31"/>
-      <c r="L81" s="31"/>
-    </row>
-    <row r="82" spans="1:12" ht="16">
-      <c r="A82" s="28" t="s">
+      <c r="E85">
+        <v>-1</v>
+      </c>
+      <c r="O85">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15" ht="16">
+      <c r="A86" s="28" t="s">
         <v>173</v>
       </c>
-      <c r="D82">
-        <v>-1</v>
-      </c>
-      <c r="L82">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="83" spans="1:12" ht="16">
-      <c r="A83" s="28" t="s">
+    </row>
+    <row r="87" spans="1:15" ht="16">
+      <c r="A87" s="28" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="84" spans="1:12" ht="16">
-      <c r="A84" s="28" t="s">
+    <row r="88" spans="1:15" ht="16">
+      <c r="A88" s="28" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="85" spans="1:12" ht="16">
-      <c r="A85" s="28" t="s">
-        <v>176</v>
-      </c>
-      <c r="D85">
-        <v>-1</v>
-      </c>
-      <c r="L85">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="86" spans="1:12" ht="16">
-      <c r="A86" s="28" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="87" spans="1:12" ht="16">
-      <c r="A87" s="28" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="88" spans="1:12" ht="16">
-      <c r="A88" s="28" t="s">
-        <v>179</v>
-      </c>
-      <c r="D88">
-        <v>-1</v>
-      </c>
-      <c r="L88">
+      <c r="E88">
+        <v>-1</v>
+      </c>
+      <c r="O88">
         <v>-1</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F1:Q1"/>
-    <mergeCell ref="R1:AC1"/>
-    <mergeCell ref="AD1:AG1"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="I1:T1"/>
+    <mergeCell ref="W1:AH1"/>
+    <mergeCell ref="AK1:AN1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -6037,58 +6094,58 @@
   <sheetData>
     <row r="1" spans="1:4" ht="21" customHeight="1">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D1" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="21" customHeight="1">
       <c r="A2" s="17" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C2" s="49" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="D2" s="48" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="21" customHeight="1">
       <c r="A3" s="17" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C3" s="49"/>
       <c r="D3" s="48"/>
     </row>
     <row r="4" spans="1:4" ht="21" customHeight="1">
       <c r="A4" s="17" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C4" s="49"/>
       <c r="D4" s="48"/>
     </row>
     <row r="5" spans="1:4" ht="21" customHeight="1">
       <c r="A5" s="18" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C5" s="49"/>
       <c r="D5" s="48"/>
@@ -6098,13 +6155,13 @@
         <v>32</v>
       </c>
       <c r="B6" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C6" s="50" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D6" s="48" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="21" customHeight="1">
@@ -6112,7 +6169,7 @@
         <v>31</v>
       </c>
       <c r="B7" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C7" s="50"/>
       <c r="D7" s="48"/>
@@ -6122,7 +6179,7 @@
         <v>30</v>
       </c>
       <c r="B8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C8" s="50"/>
       <c r="D8" s="48"/>
@@ -6132,7 +6189,7 @@
         <v>29</v>
       </c>
       <c r="B9" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C9" s="50"/>
       <c r="D9" s="48"/>
@@ -6142,7 +6199,7 @@
         <v>28</v>
       </c>
       <c r="B10" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C10" s="50"/>
       <c r="D10" s="48"/>
@@ -6152,7 +6209,7 @@
         <v>27</v>
       </c>
       <c r="B11" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C11" s="50"/>
       <c r="D11" s="48"/>
@@ -6162,7 +6219,7 @@
         <v>26</v>
       </c>
       <c r="B12" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C12" s="50"/>
       <c r="D12" s="48"/>
@@ -6172,7 +6229,7 @@
         <v>25</v>
       </c>
       <c r="B13" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C13" s="50"/>
       <c r="D13" s="48"/>
@@ -6182,17 +6239,17 @@
         <v>24</v>
       </c>
       <c r="B14" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C14" s="50"/>
       <c r="D14" s="48"/>
     </row>
     <row r="15" spans="1:4" ht="21" customHeight="1">
       <c r="A15" s="17" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B15" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C15" s="50"/>
       <c r="D15" s="48"/>
@@ -6202,7 +6259,7 @@
         <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C16" s="50"/>
       <c r="D16" s="48"/>
@@ -6212,7 +6269,7 @@
         <v>21</v>
       </c>
       <c r="B17" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C17" s="50"/>
       <c r="D17" s="48"/>
@@ -6222,10 +6279,10 @@
         <v>20</v>
       </c>
       <c r="B18" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C18" s="48" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="21" customHeight="1">
@@ -6233,7 +6290,7 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C19" s="48"/>
     </row>
@@ -6242,7 +6299,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C20" s="48"/>
     </row>
@@ -6251,7 +6308,7 @@
         <v>17</v>
       </c>
       <c r="B21" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C21" s="48"/>
     </row>
@@ -6260,7 +6317,7 @@
         <v>16</v>
       </c>
       <c r="B22" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C22" s="48"/>
     </row>
@@ -6269,7 +6326,7 @@
         <v>15</v>
       </c>
       <c r="B23" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C23" s="48"/>
     </row>
@@ -6278,7 +6335,7 @@
         <v>14</v>
       </c>
       <c r="B24" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C24" s="48"/>
     </row>
@@ -6287,7 +6344,7 @@
         <v>13</v>
       </c>
       <c r="B25" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C25" s="48"/>
     </row>
@@ -6296,7 +6353,7 @@
         <v>12</v>
       </c>
       <c r="B26" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C26" s="48"/>
     </row>
@@ -6305,7 +6362,7 @@
         <v>11</v>
       </c>
       <c r="B27" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C27" s="48"/>
     </row>
@@ -6314,7 +6371,7 @@
         <v>10</v>
       </c>
       <c r="B28" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C28" s="48"/>
     </row>
@@ -6323,7 +6380,7 @@
         <v>9</v>
       </c>
       <c r="B29" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C29" s="48"/>
     </row>
@@ -6332,13 +6389,13 @@
         <v>8</v>
       </c>
       <c r="B30" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C30" s="48" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D30" s="48" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="21" customHeight="1">
@@ -6346,7 +6403,7 @@
         <v>7</v>
       </c>
       <c r="B31" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C31" s="48"/>
       <c r="D31" s="48"/>
@@ -6356,7 +6413,7 @@
         <v>6</v>
       </c>
       <c r="B32" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C32" s="48"/>
       <c r="D32" s="48"/>
@@ -6366,7 +6423,7 @@
         <v>5</v>
       </c>
       <c r="B33" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C33" s="48"/>
       <c r="D33" s="48"/>
@@ -6390,7 +6447,7 @@
   <dimension ref="A1:AS33"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A7"/>
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -6440,139 +6497,139 @@
   <sheetData>
     <row r="1" spans="1:45" s="21" customFormat="1" ht="52.5" customHeight="1">
       <c r="A1" s="20" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B1" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="F1" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="G1" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="H1" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="I1" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="J1" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="K1" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="G1" s="21" t="s">
-        <v>108</v>
-      </c>
-      <c r="H1" s="21" t="s">
+      <c r="L1" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="M1" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="N1" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="O1" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="K1" s="21" t="s">
+      <c r="P1" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="L1" s="21" t="s">
+      <c r="Q1" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="M1" s="21" t="s">
-        <v>111</v>
-      </c>
-      <c r="N1" s="21" t="s">
+      <c r="R1" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="O1" s="21" t="s">
+      <c r="S1" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="T1" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="P1" s="21" t="s">
+      <c r="U1" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="Q1" s="21" t="s">
+      <c r="V1" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="R1" s="21" t="s">
+      <c r="W1" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="S1" s="21" t="s">
-        <v>113</v>
-      </c>
-      <c r="T1" s="21" t="s">
+      <c r="X1" s="21" t="s">
         <v>86</v>
       </c>
-      <c r="U1" s="21" t="s">
+      <c r="Y1" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="V1" s="21" t="s">
+      <c r="Z1" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="W1" s="21" t="s">
+      <c r="AA1" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB1" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC1" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="X1" s="21" t="s">
+      <c r="AD1" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="Y1" s="21" t="s">
+      <c r="AE1" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="AF1" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="Z1" s="21" t="s">
+      <c r="AG1" s="21" t="s">
+        <v>116</v>
+      </c>
+      <c r="AH1" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="AA1" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="AB1" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="AC1" s="21" t="s">
+      <c r="AI1" s="21" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ1" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="AD1" s="21" t="s">
+      <c r="AK1" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="AL1" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="AE1" s="21" t="s">
-        <v>118</v>
-      </c>
-      <c r="AF1" s="21" t="s">
+      <c r="AM1" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="AN1" s="21" t="s">
         <v>95</v>
       </c>
-      <c r="AG1" s="21" t="s">
+      <c r="AO1" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="AH1" s="21" t="s">
+      <c r="AP1" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="AI1" s="21" t="s">
+      <c r="AQ1" s="21" t="s">
         <v>121</v>
       </c>
-      <c r="AJ1" s="21" t="s">
+      <c r="AR1" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="AK1" s="21" t="s">
+      <c r="AS1" s="21" t="s">
         <v>122</v>
-      </c>
-      <c r="AL1" s="21" t="s">
-        <v>98</v>
-      </c>
-      <c r="AM1" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="AN1" s="21" t="s">
-        <v>99</v>
-      </c>
-      <c r="AO1" s="21" t="s">
-        <v>124</v>
-      </c>
-      <c r="AP1" s="21" t="s">
-        <v>100</v>
-      </c>
-      <c r="AQ1" s="21" t="s">
-        <v>125</v>
-      </c>
-      <c r="AR1" s="21" t="s">
-        <v>101</v>
-      </c>
-      <c r="AS1" s="21" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:45" ht="16">
@@ -6693,7 +6750,7 @@
     </row>
     <row r="7" spans="1:45" ht="32">
       <c r="A7" s="2" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="B7">
         <v>-1</v>
@@ -6722,7 +6779,7 @@
     </row>
     <row r="10" spans="1:45" ht="16">
       <c r="A10" s="30" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C10" s="31"/>
       <c r="D10" s="31"/>
@@ -6733,7 +6790,7 @@
     </row>
     <row r="11" spans="1:45" ht="16">
       <c r="A11" s="30" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C11" s="31"/>
       <c r="D11" s="31"/>
@@ -6744,7 +6801,7 @@
     </row>
     <row r="12" spans="1:45" ht="16">
       <c r="A12" s="30" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="D12">
         <v>-1</v>
@@ -6752,7 +6809,7 @@
     </row>
     <row r="13" spans="1:45" ht="16">
       <c r="A13" s="30" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C13" s="31"/>
       <c r="D13" s="31"/>
@@ -6763,12 +6820,12 @@
     </row>
     <row r="14" spans="1:45" ht="16">
       <c r="A14" s="30" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="15" spans="1:45" ht="16">
       <c r="A15" s="30" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C15" s="31"/>
       <c r="D15" s="31"/>
@@ -6779,12 +6836,12 @@
     </row>
     <row r="16" spans="1:45" ht="16">
       <c r="A16" s="32" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="17" spans="1:33" ht="16">
       <c r="A17" s="30" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C17" s="31"/>
       <c r="D17" s="31"/>
@@ -6795,7 +6852,7 @@
     </row>
     <row r="18" spans="1:33" ht="16">
       <c r="A18" s="30" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="D18">
         <v>-1</v>
@@ -6803,7 +6860,7 @@
     </row>
     <row r="19" spans="1:33" ht="16">
       <c r="A19" s="30" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C19" s="31"/>
       <c r="D19" s="31"/>
@@ -6812,13 +6869,13 @@
     </row>
     <row r="20" spans="1:33" ht="16">
       <c r="A20" s="30" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="D20" s="34"/>
     </row>
     <row r="21" spans="1:33" ht="16">
       <c r="A21" s="30" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="D21">
         <v>-1</v>
@@ -6826,18 +6883,18 @@
     </row>
     <row r="22" spans="1:33" ht="16">
       <c r="A22" s="28" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="23" spans="1:33" ht="16">
       <c r="A23" s="28" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="D23" s="35"/>
     </row>
     <row r="24" spans="1:33" ht="16">
       <c r="A24" s="28" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D24">
         <v>-1</v>
@@ -6845,18 +6902,18 @@
     </row>
     <row r="25" spans="1:33" ht="16">
       <c r="A25" s="28" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="26" spans="1:33" ht="16">
       <c r="A26" s="28" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D26" s="31"/>
     </row>
     <row r="27" spans="1:33" ht="16">
       <c r="A27" s="28" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="D27">
         <v>-1</v>
@@ -6864,17 +6921,17 @@
     </row>
     <row r="28" spans="1:33" ht="32">
       <c r="A28" s="28" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="29" spans="1:33" ht="32">
       <c r="A29" s="28" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="30" spans="1:33" ht="32">
       <c r="A30" s="28" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D30">
         <v>-1</v>
@@ -6882,17 +6939,17 @@
     </row>
     <row r="31" spans="1:33" ht="32">
       <c r="A31" s="28" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="32" spans="1:33" ht="32">
       <c r="A32" s="28" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="32">
       <c r="A33" s="28" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="D33">
         <v>-1</v>
@@ -6922,486 +6979,486 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B2" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B3" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C3" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C4" t="s">
         <v>102</v>
-      </c>
-      <c r="C4" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B5" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C5" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B6" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C6" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B7" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C7" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B8" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C8" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B9" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C9" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B10" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C10" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B11" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C11" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B12" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C12" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B13" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C13" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B14" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C14" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B15" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C15" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B16" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C16" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B17" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C17" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B18" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C18" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B19" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C19" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B20" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C20" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B21" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C21" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B22" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C22" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B23" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C23" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B24" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C24" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B25" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C25" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B26" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C26" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B27" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C27" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B28" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C28" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B29" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C29" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B30" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C30" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B31" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C31" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B32" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C32" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B33" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C33" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B34" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C34" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B35" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C35" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B36" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C36" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B37" t="s">
+        <v>108</v>
+      </c>
+      <c r="C37" t="s">
         <v>112</v>
-      </c>
-      <c r="C37" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B38" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C38" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B39" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C39" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B40" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C40" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B41" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C41" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B42" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C42" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B43" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C43" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B44" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C44" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -7413,8 +7470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39D49925-3FF0-9342-AD81-24B91F515069}">
   <dimension ref="A1:BD7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="AD6" sqref="AD6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Y1" sqref="Y1:Y1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -7428,31 +7485,31 @@
   <sheetData>
     <row r="1" spans="1:56" ht="16">
       <c r="A1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B1" s="41" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C1" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="38" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="D1" s="38" t="s">
+      <c r="F1" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="E1" s="38" t="s">
-        <v>44</v>
-      </c>
-      <c r="F1" s="38" t="s">
-        <v>46</v>
-      </c>
       <c r="G1" s="39" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="H1" s="43" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="I1" s="43" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="J1" s="40" t="s">
         <v>32</v>
@@ -7491,37 +7548,37 @@
         <v>21</v>
       </c>
       <c r="V1" s="40" t="s">
+        <v>182</v>
+      </c>
+      <c r="W1" s="40" t="s">
+        <v>183</v>
+      </c>
+      <c r="X1" s="40" t="s">
+        <v>184</v>
+      </c>
+      <c r="Y1" s="44" t="s">
+        <v>193</v>
+      </c>
+      <c r="Z1" s="44" t="s">
+        <v>194</v>
+      </c>
+      <c r="AA1" s="40" t="s">
+        <v>185</v>
+      </c>
+      <c r="AB1" s="40" t="s">
         <v>186</v>
       </c>
-      <c r="W1" s="40" t="s">
+      <c r="AC1" s="40" t="s">
         <v>187</v>
       </c>
-      <c r="X1" s="40" t="s">
+      <c r="AD1" s="40" t="s">
         <v>188</v>
       </c>
-      <c r="Y1" s="44" t="s">
-        <v>197</v>
-      </c>
-      <c r="Z1" s="44" t="s">
-        <v>198</v>
-      </c>
-      <c r="AA1" s="40" t="s">
+      <c r="AE1" s="40" t="s">
         <v>189</v>
       </c>
-      <c r="AB1" s="40" t="s">
-        <v>190</v>
-      </c>
-      <c r="AC1" s="40" t="s">
-        <v>191</v>
-      </c>
-      <c r="AD1" s="40" t="s">
-        <v>192</v>
-      </c>
-      <c r="AE1" s="40" t="s">
-        <v>193</v>
-      </c>
       <c r="AF1" s="45" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="AG1" s="40"/>
       <c r="AH1" s="40"/>
@@ -7659,7 +7716,7 @@
     </row>
     <row r="7" spans="1:56" ht="16">
       <c r="A7" s="2" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="B7" s="42"/>
       <c r="F7">

</xml_diff>

<commit_message>
changed implementation of Mt and Nt to use ellenburg scores - 106/190 now correct
</commit_message>
<xml_diff>
--- a/change.xlsx
+++ b/change.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elinfalla/Dropbox/2020-21/_Imperial_MSc/_Project/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37A30F6A-AA41-C44F-9EE8-D1BF34CA3872}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63A2A978-4BA5-F046-99EB-493078395EB5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="5" xr2:uid="{D6098C0C-5D8D-4C8C-96C7-825309F64318}"/>
   </bookViews>
@@ -8104,8 +8104,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3393DC69-943B-2E4A-8022-3ED8DE99B323}">
   <dimension ref="A1:AU8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
-      <selection activeCell="AC8" sqref="AC8"/>
+    <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
+      <selection activeCell="AK12" sqref="AK12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
add snail shell col to bee change spreadsheet, affected by increased agrochems
</commit_message>
<xml_diff>
--- a/change.xlsx
+++ b/change.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elinfalla/Dropbox/2020-21/_Imperial_MSc/_Project/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58C42C06-D4A8-C049-8C31-E1E8147AE78A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77E4DB78-958A-1C4E-9C6F-B0A032B09A55}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{D6098C0C-5D8D-4C8C-96C7-825309F64318}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{D6098C0C-5D8D-4C8C-96C7-825309F64318}"/>
   </bookViews>
   <sheets>
     <sheet name="pollinators" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="mammals" sheetId="3" r:id="rId3"/>
     <sheet name="mammal_key" sheetId="5" r:id="rId4"/>
     <sheet name="butterflies" sheetId="6" r:id="rId5"/>
+    <sheet name="plants" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -321,7 +322,7 @@
     Crop (grass) nest</t>
       </text>
     </comment>
-    <comment ref="AK2" authorId="29" shapeId="0" xr:uid="{2B82472E-59FF-4148-AB12-C02672624F2E}">
+    <comment ref="AL2" authorId="29" shapeId="0" xr:uid="{2B82472E-59FF-4148-AB12-C02672624F2E}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -329,7 +330,7 @@
     Hedge - plants associated with damp areas specifically</t>
       </text>
     </comment>
-    <comment ref="AL2" authorId="30" shapeId="0" xr:uid="{74099FC7-8ABC-4BCA-B048-586D8C2AB079}">
+    <comment ref="AM2" authorId="30" shapeId="0" xr:uid="{74099FC7-8ABC-4BCA-B048-586D8C2AB079}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -337,7 +338,7 @@
     Margin - plants associated with damp areas specifically</t>
       </text>
     </comment>
-    <comment ref="AM2" authorId="31" shapeId="0" xr:uid="{48C3A0E7-35F7-49D1-B02F-BFD8904E48CB}">
+    <comment ref="AN2" authorId="31" shapeId="0" xr:uid="{48C3A0E7-35F7-49D1-B02F-BFD8904E48CB}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -345,7 +346,7 @@
     Crop (arable) - plants associated with damp areas specifically</t>
       </text>
     </comment>
-    <comment ref="AN2" authorId="32" shapeId="0" xr:uid="{90E5597C-0F3C-4878-B496-32CD19452B20}">
+    <comment ref="AO2" authorId="32" shapeId="0" xr:uid="{90E5597C-0F3C-4878-B496-32CD19452B20}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -3465,8 +3466,26 @@
 </comments>
 </file>
 
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={97EF5719-78D5-F14B-8F08-DD618AD6AD0B}</author>
+  </authors>
+  <commentList>
+    <comment ref="AA3" authorId="0" shapeId="0" xr:uid="{97EF5719-78D5-F14B-8F08-DD618AD6AD0B}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    for autumn germinating species only</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="243">
   <si>
     <t>hay_sil</t>
   </si>
@@ -4151,12 +4170,144 @@
   <si>
     <t>inc_stocking</t>
   </si>
+  <si>
+    <t>Habitats</t>
+  </si>
+  <si>
+    <t>Germination period</t>
+  </si>
+  <si>
+    <t>Flowering period</t>
+  </si>
+  <si>
+    <t>Herbicide susceptibility</t>
+  </si>
+  <si>
+    <t>Soil moisture affinity</t>
+  </si>
+  <si>
+    <t>Nitrogen affinity</t>
+  </si>
+  <si>
+    <t>germ_start</t>
+  </si>
+  <si>
+    <t>H_G_Sp</t>
+  </si>
+  <si>
+    <t>H_G_Au</t>
+  </si>
+  <si>
+    <t>M_G_Sp</t>
+  </si>
+  <si>
+    <t>M_G_Au</t>
+  </si>
+  <si>
+    <t>C_G_Sp</t>
+  </si>
+  <si>
+    <t>C_G_Au</t>
+  </si>
+  <si>
+    <t>germ_end</t>
+  </si>
+  <si>
+    <t>flower_start</t>
+  </si>
+  <si>
+    <t>H_F_April</t>
+  </si>
+  <si>
+    <t>H_F_May</t>
+  </si>
+  <si>
+    <t>H_F_June</t>
+  </si>
+  <si>
+    <t>H_F_July</t>
+  </si>
+  <si>
+    <t>M_F_April</t>
+  </si>
+  <si>
+    <t>M_F_May</t>
+  </si>
+  <si>
+    <t>M_F_June</t>
+  </si>
+  <si>
+    <t>M_F_July</t>
+  </si>
+  <si>
+    <t>C_F_April</t>
+  </si>
+  <si>
+    <t>C_F_May</t>
+  </si>
+  <si>
+    <t>C_F_June</t>
+  </si>
+  <si>
+    <t>C_F_July</t>
+  </si>
+  <si>
+    <t>flower_end</t>
+  </si>
+  <si>
+    <t>herbi_start</t>
+  </si>
+  <si>
+    <t>H_Herbi</t>
+  </si>
+  <si>
+    <t>M_Herbi</t>
+  </si>
+  <si>
+    <t>C_Herbi</t>
+  </si>
+  <si>
+    <t>herbi_end</t>
+  </si>
+  <si>
+    <t>moist_start</t>
+  </si>
+  <si>
+    <t>H_Moisture</t>
+  </si>
+  <si>
+    <t>M_Moisture</t>
+  </si>
+  <si>
+    <t>C_Moisture</t>
+  </si>
+  <si>
+    <t>moist_end</t>
+  </si>
+  <si>
+    <t>nitro_start</t>
+  </si>
+  <si>
+    <t>H_Nitrogen</t>
+  </si>
+  <si>
+    <t>M_Nitrogen</t>
+  </si>
+  <si>
+    <t>C_Nitrogen</t>
+  </si>
+  <si>
+    <t>nitro_end</t>
+  </si>
+  <si>
+    <t>CG_N_Snail shells</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4272,8 +4423,19 @@
       <family val="3"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="27">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4328,8 +4490,110 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -4366,11 +4630,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -4484,6 +4768,70 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4496,16 +4844,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4533,6 +4898,7 @@
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <person displayName="Alexa Varah" id="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" userId="Alexa Varah" providerId="None"/>
+  <person displayName="Falla, Elin" id="{8B4A21F5-18CE-8F41-9706-AB9C540A7308}" userId="S::ef16@ic.ac.uk::6f3a10e9-5277-43c9-a417-47b31449ff76" providerId="AD"/>
 </personList>
 </file>
 
@@ -4925,16 +5291,16 @@
   <threadedComment ref="AH2" dT="2020-06-17T10:28:24.74" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{E625A537-1514-4930-ADE3-685B712C12DD}">
     <text>Crop (grass) nest</text>
   </threadedComment>
-  <threadedComment ref="AK2" dT="2020-06-17T10:30:15.35" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{2B82472E-59FF-4148-AB12-C02672624F2E}">
+  <threadedComment ref="AL2" dT="2020-06-17T10:30:15.35" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{2B82472E-59FF-4148-AB12-C02672624F2E}">
     <text>Hedge - plants associated with damp areas specifically</text>
   </threadedComment>
-  <threadedComment ref="AL2" dT="2020-06-17T10:30:22.42" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{74099FC7-8ABC-4BCA-B048-586D8C2AB079}">
+  <threadedComment ref="AM2" dT="2020-06-17T10:30:22.42" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{74099FC7-8ABC-4BCA-B048-586D8C2AB079}">
     <text>Margin - plants associated with damp areas specifically</text>
   </threadedComment>
-  <threadedComment ref="AM2" dT="2020-06-17T10:30:30.20" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{48C3A0E7-35F7-49D1-B02F-BFD8904E48CB}">
+  <threadedComment ref="AN2" dT="2020-06-17T10:30:30.20" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{48C3A0E7-35F7-49D1-B02F-BFD8904E48CB}">
     <text>Crop (arable) - plants associated with damp areas specifically</text>
   </threadedComment>
-  <threadedComment ref="AN2" dT="2020-06-17T10:30:37.43" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{90E5597C-0F3C-4878-B496-32CD19452B20}">
+  <threadedComment ref="AO2" dT="2020-06-17T10:30:37.43" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{90E5597C-0F3C-4878-B496-32CD19452B20}">
     <text>Crop (grass) - plants associated with damp areas specifically</text>
   </threadedComment>
   <threadedComment ref="E3" dT="2020-09-10T14:58:25.44" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{C1BDF87D-1D41-44ED-9DB5-82CE7A80DFFC}">
@@ -4969,13 +5335,21 @@
 </ThreadedComments>
 </file>
 
+<file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="AA3" dT="2021-05-23T20:43:45.94" personId="{8B4A21F5-18CE-8F41-9706-AB9C540A7308}" id="{97EF5719-78D5-F14B-8F08-DD618AD6AD0B}">
+    <text>for autumn germinating species only</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64F6D29A-951C-4B7B-AAD7-CC63BC8BEE38}">
-  <dimension ref="A1:AO88"/>
+  <dimension ref="A1:AP88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AB11" sqref="AB11"/>
+      <selection pane="bottomLeft" activeCell="AI4" sqref="AI4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -4990,60 +5364,61 @@
     <col min="24" max="24" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="25" max="31" width="6.6640625" customWidth="1"/>
     <col min="32" max="32" width="8.1640625" customWidth="1"/>
-    <col min="33" max="34" width="6.6640625" customWidth="1"/>
-    <col min="35" max="36" width="6.6640625" style="41" customWidth="1"/>
-    <col min="37" max="40" width="3.33203125" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="8.83203125" style="41"/>
+    <col min="33" max="35" width="6.6640625" customWidth="1"/>
+    <col min="36" max="37" width="6.6640625" style="41" customWidth="1"/>
+    <col min="38" max="41" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="8.83203125" style="41"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" s="27" customFormat="1" ht="32.75" customHeight="1">
+    <row r="1" spans="1:42" s="27" customFormat="1" ht="32.75" customHeight="1">
       <c r="A1" s="26"/>
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="76" t="s">
         <v>129</v>
       </c>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="I1" s="46" t="s">
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="I1" s="76" t="s">
         <v>66</v>
       </c>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="46"/>
-      <c r="P1" s="46"/>
-      <c r="Q1" s="46"/>
-      <c r="R1" s="46"/>
-      <c r="S1" s="46"/>
-      <c r="T1" s="46"/>
+      <c r="J1" s="76"/>
+      <c r="K1" s="76"/>
+      <c r="L1" s="76"/>
+      <c r="M1" s="76"/>
+      <c r="N1" s="76"/>
+      <c r="O1" s="76"/>
+      <c r="P1" s="76"/>
+      <c r="Q1" s="76"/>
+      <c r="R1" s="76"/>
+      <c r="S1" s="76"/>
+      <c r="T1" s="76"/>
       <c r="V1" s="44"/>
-      <c r="W1" s="46" t="s">
+      <c r="W1" s="76" t="s">
         <v>134</v>
       </c>
-      <c r="X1" s="46"/>
-      <c r="Y1" s="46"/>
-      <c r="Z1" s="46"/>
-      <c r="AA1" s="46"/>
-      <c r="AB1" s="46"/>
-      <c r="AC1" s="46"/>
-      <c r="AD1" s="46"/>
-      <c r="AE1" s="46"/>
-      <c r="AF1" s="46"/>
-      <c r="AG1" s="46"/>
-      <c r="AH1" s="46"/>
-      <c r="AI1" s="51"/>
-      <c r="AJ1" s="51"/>
-      <c r="AK1" s="47" t="s">
+      <c r="X1" s="76"/>
+      <c r="Y1" s="76"/>
+      <c r="Z1" s="76"/>
+      <c r="AA1" s="76"/>
+      <c r="AB1" s="76"/>
+      <c r="AC1" s="76"/>
+      <c r="AD1" s="76"/>
+      <c r="AE1" s="76"/>
+      <c r="AF1" s="76"/>
+      <c r="AG1" s="76"/>
+      <c r="AH1" s="76"/>
+      <c r="AI1" s="46"/>
+      <c r="AJ1" s="47"/>
+      <c r="AK1" s="47"/>
+      <c r="AL1" s="77" t="s">
         <v>135</v>
       </c>
-      <c r="AL1" s="47"/>
-      <c r="AM1" s="47"/>
-      <c r="AN1" s="47"/>
-      <c r="AO1" s="53"/>
-    </row>
-    <row r="2" spans="1:41" s="4" customFormat="1" ht="114.5" customHeight="1">
+      <c r="AM1" s="77"/>
+      <c r="AN1" s="77"/>
+      <c r="AO1" s="77"/>
+      <c r="AP1" s="49"/>
+    </row>
+    <row r="2" spans="1:42" s="4" customFormat="1" ht="114.5" customHeight="1">
       <c r="A2" s="14" t="s">
         <v>33</v>
       </c>
@@ -5146,29 +5521,32 @@
       <c r="AH2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="AI2" s="52" t="s">
+      <c r="AI2" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="AJ2" s="48" t="s">
         <v>197</v>
       </c>
-      <c r="AJ2" s="52" t="s">
+      <c r="AK2" s="48" t="s">
         <v>194</v>
       </c>
-      <c r="AK2" s="5" t="s">
+      <c r="AL2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="AL2" s="5" t="s">
+      <c r="AM2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="AM2" s="5" t="s">
+      <c r="AN2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="AN2" s="5" t="s">
+      <c r="AO2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="AO2" s="54" t="s">
+      <c r="AP2" s="50" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="3" spans="1:41" ht="16">
+    <row r="3" spans="1:42" ht="16">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -5181,7 +5559,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="4" spans="1:41" ht="16">
+    <row r="4" spans="1:42" ht="16">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -5192,8 +5570,11 @@
       <c r="F4" s="25">
         <v>-1</v>
       </c>
-    </row>
-    <row r="5" spans="1:41" ht="16">
+      <c r="AI4" s="37">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:42" ht="16">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -5216,11 +5597,14 @@
       <c r="N5">
         <v>-1</v>
       </c>
+      <c r="X5" s="37">
+        <v>-1</v>
+      </c>
       <c r="AA5">
         <v>-1</v>
       </c>
     </row>
-    <row r="6" spans="1:41" ht="16">
+    <row r="6" spans="1:42" ht="16">
       <c r="A6" s="2" t="s">
         <v>1</v>
       </c>
@@ -5234,7 +5618,7 @@
       <c r="N6">
         <v>-1</v>
       </c>
-      <c r="AK6">
+      <c r="AA6" s="37">
         <v>-1</v>
       </c>
       <c r="AL6">
@@ -5246,8 +5630,11 @@
       <c r="AN6">
         <v>-1</v>
       </c>
-    </row>
-    <row r="7" spans="1:41" ht="16">
+      <c r="AO6">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:42" ht="16">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
@@ -5268,7 +5655,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="8" spans="1:41" ht="16">
+    <row r="8" spans="1:42" ht="16">
       <c r="A8" s="2" t="s">
         <v>198</v>
       </c>
@@ -5282,21 +5669,21 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="9" spans="1:41">
+    <row r="9" spans="1:42">
       <c r="A9" s="2"/>
     </row>
-    <row r="10" spans="1:41">
+    <row r="10" spans="1:42">
       <c r="A10" s="24"/>
       <c r="C10" s="23"/>
     </row>
-    <row r="11" spans="1:41">
+    <row r="11" spans="1:42">
       <c r="A11" s="24"/>
       <c r="C11" s="22"/>
     </row>
-    <row r="12" spans="1:41">
+    <row r="12" spans="1:42">
       <c r="A12" s="2"/>
     </row>
-    <row r="13" spans="1:41" ht="16">
+    <row r="13" spans="1:42" ht="16">
       <c r="A13" s="2" t="s">
         <v>124</v>
       </c>
@@ -5307,7 +5694,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:41" ht="16">
+    <row r="14" spans="1:42" ht="16">
       <c r="A14" s="2" t="s">
         <v>125</v>
       </c>
@@ -5318,10 +5705,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:41">
+    <row r="15" spans="1:42">
       <c r="A15" s="2"/>
     </row>
-    <row r="16" spans="1:41">
+    <row r="16" spans="1:42">
       <c r="A16" s="2"/>
     </row>
     <row r="17" spans="1:20" ht="16">
@@ -6070,7 +6457,7 @@
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="I1:T1"/>
     <mergeCell ref="W1:AH1"/>
-    <mergeCell ref="AK1:AN1"/>
+    <mergeCell ref="AL1:AO1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -6113,10 +6500,10 @@
       <c r="B2" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="49" t="s">
+      <c r="C2" s="79" t="s">
         <v>131</v>
       </c>
-      <c r="D2" s="48" t="s">
+      <c r="D2" s="78" t="s">
         <v>127</v>
       </c>
     </row>
@@ -6127,8 +6514,8 @@
       <c r="B3" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="49"/>
-      <c r="D3" s="48"/>
+      <c r="C3" s="79"/>
+      <c r="D3" s="78"/>
     </row>
     <row r="4" spans="1:4" ht="21" customHeight="1">
       <c r="A4" s="17" t="s">
@@ -6137,8 +6524,8 @@
       <c r="B4" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="49"/>
-      <c r="D4" s="48"/>
+      <c r="C4" s="79"/>
+      <c r="D4" s="78"/>
     </row>
     <row r="5" spans="1:4" ht="21" customHeight="1">
       <c r="A5" s="18" t="s">
@@ -6147,8 +6534,8 @@
       <c r="B5" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="C5" s="49"/>
-      <c r="D5" s="48"/>
+      <c r="C5" s="79"/>
+      <c r="D5" s="78"/>
     </row>
     <row r="6" spans="1:4" ht="21" customHeight="1">
       <c r="A6" s="17" t="s">
@@ -6157,10 +6544,10 @@
       <c r="B6" t="s">
         <v>44</v>
       </c>
-      <c r="C6" s="50" t="s">
+      <c r="C6" s="80" t="s">
         <v>132</v>
       </c>
-      <c r="D6" s="48" t="s">
+      <c r="D6" s="78" t="s">
         <v>128</v>
       </c>
     </row>
@@ -6171,8 +6558,8 @@
       <c r="B7" t="s">
         <v>45</v>
       </c>
-      <c r="C7" s="50"/>
-      <c r="D7" s="48"/>
+      <c r="C7" s="80"/>
+      <c r="D7" s="78"/>
     </row>
     <row r="8" spans="1:4" ht="21" customHeight="1">
       <c r="A8" s="17" t="s">
@@ -6181,8 +6568,8 @@
       <c r="B8" t="s">
         <v>46</v>
       </c>
-      <c r="C8" s="50"/>
-      <c r="D8" s="48"/>
+      <c r="C8" s="80"/>
+      <c r="D8" s="78"/>
     </row>
     <row r="9" spans="1:4" ht="21" customHeight="1">
       <c r="A9" s="17" t="s">
@@ -6191,8 +6578,8 @@
       <c r="B9" t="s">
         <v>47</v>
       </c>
-      <c r="C9" s="50"/>
-      <c r="D9" s="48"/>
+      <c r="C9" s="80"/>
+      <c r="D9" s="78"/>
     </row>
     <row r="10" spans="1:4" ht="21" customHeight="1">
       <c r="A10" s="17" t="s">
@@ -6201,8 +6588,8 @@
       <c r="B10" t="s">
         <v>48</v>
       </c>
-      <c r="C10" s="50"/>
-      <c r="D10" s="48"/>
+      <c r="C10" s="80"/>
+      <c r="D10" s="78"/>
     </row>
     <row r="11" spans="1:4" ht="21" customHeight="1">
       <c r="A11" s="17" t="s">
@@ -6211,8 +6598,8 @@
       <c r="B11" t="s">
         <v>49</v>
       </c>
-      <c r="C11" s="50"/>
-      <c r="D11" s="48"/>
+      <c r="C11" s="80"/>
+      <c r="D11" s="78"/>
     </row>
     <row r="12" spans="1:4" ht="21" customHeight="1">
       <c r="A12" s="17" t="s">
@@ -6221,8 +6608,8 @@
       <c r="B12" t="s">
         <v>50</v>
       </c>
-      <c r="C12" s="50"/>
-      <c r="D12" s="48"/>
+      <c r="C12" s="80"/>
+      <c r="D12" s="78"/>
     </row>
     <row r="13" spans="1:4" ht="21" customHeight="1">
       <c r="A13" s="17" t="s">
@@ -6231,8 +6618,8 @@
       <c r="B13" t="s">
         <v>51</v>
       </c>
-      <c r="C13" s="50"/>
-      <c r="D13" s="48"/>
+      <c r="C13" s="80"/>
+      <c r="D13" s="78"/>
     </row>
     <row r="14" spans="1:4" ht="21" customHeight="1">
       <c r="A14" s="17" t="s">
@@ -6241,8 +6628,8 @@
       <c r="B14" t="s">
         <v>52</v>
       </c>
-      <c r="C14" s="50"/>
-      <c r="D14" s="48"/>
+      <c r="C14" s="80"/>
+      <c r="D14" s="78"/>
     </row>
     <row r="15" spans="1:4" ht="21" customHeight="1">
       <c r="A15" s="17" t="s">
@@ -6251,8 +6638,8 @@
       <c r="B15" t="s">
         <v>54</v>
       </c>
-      <c r="C15" s="50"/>
-      <c r="D15" s="48"/>
+      <c r="C15" s="80"/>
+      <c r="D15" s="78"/>
     </row>
     <row r="16" spans="1:4" ht="21" customHeight="1">
       <c r="A16" s="17" t="s">
@@ -6261,8 +6648,8 @@
       <c r="B16" t="s">
         <v>55</v>
       </c>
-      <c r="C16" s="50"/>
-      <c r="D16" s="48"/>
+      <c r="C16" s="80"/>
+      <c r="D16" s="78"/>
     </row>
     <row r="17" spans="1:4" ht="21" customHeight="1">
       <c r="A17" s="17" t="s">
@@ -6271,8 +6658,8 @@
       <c r="B17" t="s">
         <v>56</v>
       </c>
-      <c r="C17" s="50"/>
-      <c r="D17" s="48"/>
+      <c r="C17" s="80"/>
+      <c r="D17" s="78"/>
     </row>
     <row r="18" spans="1:4" ht="21" customHeight="1">
       <c r="A18" s="17" t="s">
@@ -6281,7 +6668,7 @@
       <c r="B18" t="s">
         <v>57</v>
       </c>
-      <c r="C18" s="48" t="s">
+      <c r="C18" s="78" t="s">
         <v>134</v>
       </c>
     </row>
@@ -6292,7 +6679,7 @@
       <c r="B19" t="s">
         <v>57</v>
       </c>
-      <c r="C19" s="48"/>
+      <c r="C19" s="78"/>
     </row>
     <row r="20" spans="1:4" ht="21" customHeight="1">
       <c r="A20" s="18" t="s">
@@ -6301,7 +6688,7 @@
       <c r="B20" t="s">
         <v>57</v>
       </c>
-      <c r="C20" s="48"/>
+      <c r="C20" s="78"/>
     </row>
     <row r="21" spans="1:4" ht="21" customHeight="1">
       <c r="A21" s="17" t="s">
@@ -6310,7 +6697,7 @@
       <c r="B21" t="s">
         <v>58</v>
       </c>
-      <c r="C21" s="48"/>
+      <c r="C21" s="78"/>
     </row>
     <row r="22" spans="1:4" ht="21" customHeight="1">
       <c r="A22" s="17" t="s">
@@ -6319,7 +6706,7 @@
       <c r="B22" t="s">
         <v>58</v>
       </c>
-      <c r="C22" s="48"/>
+      <c r="C22" s="78"/>
     </row>
     <row r="23" spans="1:4" ht="21" customHeight="1">
       <c r="A23" s="17" t="s">
@@ -6328,7 +6715,7 @@
       <c r="B23" t="s">
         <v>58</v>
       </c>
-      <c r="C23" s="48"/>
+      <c r="C23" s="78"/>
     </row>
     <row r="24" spans="1:4" ht="21" customHeight="1">
       <c r="A24" s="18" t="s">
@@ -6337,7 +6724,7 @@
       <c r="B24" t="s">
         <v>58</v>
       </c>
-      <c r="C24" s="48"/>
+      <c r="C24" s="78"/>
     </row>
     <row r="25" spans="1:4" ht="21" customHeight="1">
       <c r="A25" s="18" t="s">
@@ -6346,7 +6733,7 @@
       <c r="B25" t="s">
         <v>59</v>
       </c>
-      <c r="C25" s="48"/>
+      <c r="C25" s="78"/>
     </row>
     <row r="26" spans="1:4" ht="21" customHeight="1">
       <c r="A26" s="17" t="s">
@@ -6355,7 +6742,7 @@
       <c r="B26" t="s">
         <v>60</v>
       </c>
-      <c r="C26" s="48"/>
+      <c r="C26" s="78"/>
     </row>
     <row r="27" spans="1:4" ht="21" customHeight="1">
       <c r="A27" s="17" t="s">
@@ -6364,7 +6751,7 @@
       <c r="B27" t="s">
         <v>60</v>
       </c>
-      <c r="C27" s="48"/>
+      <c r="C27" s="78"/>
     </row>
     <row r="28" spans="1:4" ht="21" customHeight="1">
       <c r="A28" s="17" t="s">
@@ -6373,7 +6760,7 @@
       <c r="B28" t="s">
         <v>60</v>
       </c>
-      <c r="C28" s="48"/>
+      <c r="C28" s="78"/>
     </row>
     <row r="29" spans="1:4" ht="21" customHeight="1">
       <c r="A29" s="18" t="s">
@@ -6382,7 +6769,7 @@
       <c r="B29" t="s">
         <v>60</v>
       </c>
-      <c r="C29" s="48"/>
+      <c r="C29" s="78"/>
     </row>
     <row r="30" spans="1:4" ht="21" customHeight="1">
       <c r="A30" s="18" t="s">
@@ -6391,10 +6778,10 @@
       <c r="B30" t="s">
         <v>61</v>
       </c>
-      <c r="C30" s="48" t="s">
+      <c r="C30" s="78" t="s">
         <v>130</v>
       </c>
-      <c r="D30" s="48" t="s">
+      <c r="D30" s="78" t="s">
         <v>133</v>
       </c>
     </row>
@@ -6405,8 +6792,8 @@
       <c r="B31" t="s">
         <v>62</v>
       </c>
-      <c r="C31" s="48"/>
-      <c r="D31" s="48"/>
+      <c r="C31" s="78"/>
+      <c r="D31" s="78"/>
     </row>
     <row r="32" spans="1:4" ht="21" customHeight="1">
       <c r="A32" s="18" t="s">
@@ -6415,8 +6802,8 @@
       <c r="B32" t="s">
         <v>63</v>
       </c>
-      <c r="C32" s="48"/>
-      <c r="D32" s="48"/>
+      <c r="C32" s="78"/>
+      <c r="D32" s="78"/>
     </row>
     <row r="33" spans="1:4" ht="21" customHeight="1">
       <c r="A33" s="18" t="s">
@@ -6425,8 +6812,8 @@
       <c r="B33" t="s">
         <v>64</v>
       </c>
-      <c r="C33" s="48"/>
-      <c r="D33" s="48"/>
+      <c r="C33" s="78"/>
+      <c r="D33" s="78"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -7470,9 +7857,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39D49925-3FF0-9342-AD81-24B91F515069}">
   <dimension ref="A1:BD7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Y1" sqref="Y1:Y1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
@@ -7726,4 +8111,339 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3393DC69-943B-2E4A-8022-3ED8DE99B323}">
+  <dimension ref="A1:AU8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:47">
+      <c r="A1" s="51"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="81" t="s">
+        <v>199</v>
+      </c>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="82" t="s">
+        <v>200</v>
+      </c>
+      <c r="I1" s="82"/>
+      <c r="J1" s="82"/>
+      <c r="K1" s="82"/>
+      <c r="L1" s="82"/>
+      <c r="M1" s="82"/>
+      <c r="N1" s="53"/>
+      <c r="O1" s="53"/>
+      <c r="P1" s="83" t="s">
+        <v>201</v>
+      </c>
+      <c r="Q1" s="83"/>
+      <c r="R1" s="83"/>
+      <c r="S1" s="83"/>
+      <c r="T1" s="83"/>
+      <c r="U1" s="83"/>
+      <c r="V1" s="83"/>
+      <c r="W1" s="83"/>
+      <c r="X1" s="83"/>
+      <c r="Y1" s="83"/>
+      <c r="Z1" s="83"/>
+      <c r="AA1" s="83"/>
+      <c r="AB1" s="53"/>
+      <c r="AC1" s="53"/>
+      <c r="AD1" s="84" t="s">
+        <v>202</v>
+      </c>
+      <c r="AE1" s="85"/>
+      <c r="AF1" s="85"/>
+      <c r="AG1" s="53"/>
+      <c r="AH1" s="53"/>
+      <c r="AI1" s="86" t="s">
+        <v>203</v>
+      </c>
+      <c r="AJ1" s="87"/>
+      <c r="AK1" s="87"/>
+      <c r="AL1" s="53"/>
+      <c r="AM1" s="53"/>
+      <c r="AN1" s="88" t="s">
+        <v>204</v>
+      </c>
+      <c r="AO1" s="89"/>
+      <c r="AP1" s="89"/>
+      <c r="AQ1" s="37"/>
+      <c r="AR1" s="19"/>
+      <c r="AU1" s="19"/>
+    </row>
+    <row r="2" spans="1:47" ht="16" thickBot="1">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="54" t="s">
+        <v>190</v>
+      </c>
+      <c r="C2" s="55" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="56" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" s="57" t="s">
+        <v>88</v>
+      </c>
+      <c r="F2" s="58" t="s">
+        <v>191</v>
+      </c>
+      <c r="G2" s="58" t="s">
+        <v>205</v>
+      </c>
+      <c r="H2" s="59" t="s">
+        <v>206</v>
+      </c>
+      <c r="I2" s="60" t="s">
+        <v>207</v>
+      </c>
+      <c r="J2" s="61" t="s">
+        <v>208</v>
+      </c>
+      <c r="K2" s="60" t="s">
+        <v>209</v>
+      </c>
+      <c r="L2" s="61" t="s">
+        <v>210</v>
+      </c>
+      <c r="M2" s="60" t="s">
+        <v>211</v>
+      </c>
+      <c r="N2" s="58" t="s">
+        <v>212</v>
+      </c>
+      <c r="O2" s="58" t="s">
+        <v>213</v>
+      </c>
+      <c r="P2" s="62" t="s">
+        <v>214</v>
+      </c>
+      <c r="Q2" s="63" t="s">
+        <v>215</v>
+      </c>
+      <c r="R2" s="64" t="s">
+        <v>216</v>
+      </c>
+      <c r="S2" s="63" t="s">
+        <v>217</v>
+      </c>
+      <c r="T2" s="62" t="s">
+        <v>218</v>
+      </c>
+      <c r="U2" s="63" t="s">
+        <v>219</v>
+      </c>
+      <c r="V2" s="64" t="s">
+        <v>220</v>
+      </c>
+      <c r="W2" s="63" t="s">
+        <v>221</v>
+      </c>
+      <c r="X2" s="62" t="s">
+        <v>222</v>
+      </c>
+      <c r="Y2" s="63" t="s">
+        <v>223</v>
+      </c>
+      <c r="Z2" s="64" t="s">
+        <v>224</v>
+      </c>
+      <c r="AA2" s="63" t="s">
+        <v>225</v>
+      </c>
+      <c r="AB2" s="58" t="s">
+        <v>226</v>
+      </c>
+      <c r="AC2" s="58" t="s">
+        <v>227</v>
+      </c>
+      <c r="AD2" s="65" t="s">
+        <v>228</v>
+      </c>
+      <c r="AE2" s="66" t="s">
+        <v>229</v>
+      </c>
+      <c r="AF2" s="67" t="s">
+        <v>230</v>
+      </c>
+      <c r="AG2" s="58" t="s">
+        <v>231</v>
+      </c>
+      <c r="AH2" s="58" t="s">
+        <v>232</v>
+      </c>
+      <c r="AI2" s="68" t="s">
+        <v>233</v>
+      </c>
+      <c r="AJ2" s="69" t="s">
+        <v>234</v>
+      </c>
+      <c r="AK2" s="70" t="s">
+        <v>235</v>
+      </c>
+      <c r="AL2" s="58" t="s">
+        <v>236</v>
+      </c>
+      <c r="AM2" s="58" t="s">
+        <v>237</v>
+      </c>
+      <c r="AN2" s="71" t="s">
+        <v>238</v>
+      </c>
+      <c r="AO2" s="72" t="s">
+        <v>239</v>
+      </c>
+      <c r="AP2" s="73" t="s">
+        <v>240</v>
+      </c>
+      <c r="AQ2" s="37" t="s">
+        <v>241</v>
+      </c>
+      <c r="AR2" s="19"/>
+      <c r="AU2" s="19"/>
+    </row>
+    <row r="3" spans="1:47" ht="16">
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L3">
+        <v>-1</v>
+      </c>
+      <c r="AA3" s="74">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:47" ht="16">
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="X4">
+        <v>-1</v>
+      </c>
+      <c r="Y4">
+        <v>-1</v>
+      </c>
+      <c r="Z4">
+        <v>-1</v>
+      </c>
+      <c r="AA4">
+        <v>-1</v>
+      </c>
+      <c r="AN4" s="75"/>
+      <c r="AO4" s="75"/>
+      <c r="AP4" s="74">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:47" ht="16">
+      <c r="A5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <v>-1</v>
+      </c>
+      <c r="I5">
+        <v>-1</v>
+      </c>
+      <c r="J5">
+        <v>-1</v>
+      </c>
+      <c r="K5">
+        <v>-1</v>
+      </c>
+      <c r="P5">
+        <v>-1</v>
+      </c>
+      <c r="Q5">
+        <v>-1</v>
+      </c>
+      <c r="R5">
+        <v>-1</v>
+      </c>
+      <c r="S5">
+        <v>-1</v>
+      </c>
+      <c r="T5">
+        <v>-1</v>
+      </c>
+      <c r="U5">
+        <v>-1</v>
+      </c>
+      <c r="V5">
+        <v>-1</v>
+      </c>
+      <c r="W5">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:47" ht="16">
+      <c r="A6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>-1</v>
+      </c>
+      <c r="K6">
+        <v>-1</v>
+      </c>
+      <c r="T6">
+        <v>-1</v>
+      </c>
+      <c r="U6">
+        <v>-1</v>
+      </c>
+      <c r="V6">
+        <v>-1</v>
+      </c>
+      <c r="W6">
+        <v>-1</v>
+      </c>
+      <c r="AI6" s="74">
+        <v>-1</v>
+      </c>
+      <c r="AJ6" s="74">
+        <v>-1</v>
+      </c>
+      <c r="AK6" s="74">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:47" ht="16">
+      <c r="A7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA7">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:47" ht="16">
+      <c r="A8" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="AN1:AP1"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="H1:M1"/>
+    <mergeCell ref="P1:AA1"/>
+    <mergeCell ref="AD1:AF1"/>
+    <mergeCell ref="AI1:AK1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added Margin snail shell as nesting site to reqs and change spreadsheets,, only used by Osmia bicolor
</commit_message>
<xml_diff>
--- a/change.xlsx
+++ b/change.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elinfalla/Dropbox/2020-21/_Imperial_MSc/_Project/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77E4DB78-958A-1C4E-9C6F-B0A032B09A55}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{251682AE-C3DD-414E-BDDC-E65E4BDFF8C7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{D6098C0C-5D8D-4C8C-96C7-825309F64318}"/>
   </bookViews>
@@ -282,7 +282,7 @@
     Margin nest</t>
       </text>
     </comment>
-    <comment ref="AD2" authorId="24" shapeId="0" xr:uid="{61328AAB-8080-40A5-BB72-DE3F063064D6}">
+    <comment ref="AE2" authorId="24" shapeId="0" xr:uid="{61328AAB-8080-40A5-BB72-DE3F063064D6}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -290,7 +290,7 @@
     Crop (arable) nest</t>
       </text>
     </comment>
-    <comment ref="AE2" authorId="25" shapeId="0" xr:uid="{08D8BC3C-7DE2-46DE-A501-79F9B77FC5A6}">
+    <comment ref="AF2" authorId="25" shapeId="0" xr:uid="{08D8BC3C-7DE2-46DE-A501-79F9B77FC5A6}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -298,7 +298,7 @@
     Crop (grass) nest</t>
       </text>
     </comment>
-    <comment ref="AF2" authorId="26" shapeId="0" xr:uid="{60F49050-15F0-4A01-B60D-D08CFC1500EA}">
+    <comment ref="AG2" authorId="26" shapeId="0" xr:uid="{60F49050-15F0-4A01-B60D-D08CFC1500EA}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -306,7 +306,7 @@
     Crop (grass) nest</t>
       </text>
     </comment>
-    <comment ref="AG2" authorId="27" shapeId="0" xr:uid="{53B38088-2842-4886-AD04-FB278DF6E6D5}">
+    <comment ref="AH2" authorId="27" shapeId="0" xr:uid="{53B38088-2842-4886-AD04-FB278DF6E6D5}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -314,7 +314,7 @@
     Crop (grass) nest</t>
       </text>
     </comment>
-    <comment ref="AH2" authorId="28" shapeId="0" xr:uid="{E625A537-1514-4930-ADE3-685B712C12DD}">
+    <comment ref="AI2" authorId="28" shapeId="0" xr:uid="{E625A537-1514-4930-ADE3-685B712C12DD}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -322,7 +322,7 @@
     Crop (grass) nest</t>
       </text>
     </comment>
-    <comment ref="AL2" authorId="29" shapeId="0" xr:uid="{2B82472E-59FF-4148-AB12-C02672624F2E}">
+    <comment ref="AM2" authorId="29" shapeId="0" xr:uid="{2B82472E-59FF-4148-AB12-C02672624F2E}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -330,7 +330,7 @@
     Hedge - plants associated with damp areas specifically</t>
       </text>
     </comment>
-    <comment ref="AM2" authorId="30" shapeId="0" xr:uid="{74099FC7-8ABC-4BCA-B048-586D8C2AB079}">
+    <comment ref="AN2" authorId="30" shapeId="0" xr:uid="{74099FC7-8ABC-4BCA-B048-586D8C2AB079}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -338,7 +338,7 @@
     Margin - plants associated with damp areas specifically</t>
       </text>
     </comment>
-    <comment ref="AN2" authorId="31" shapeId="0" xr:uid="{48C3A0E7-35F7-49D1-B02F-BFD8904E48CB}">
+    <comment ref="AO2" authorId="31" shapeId="0" xr:uid="{48C3A0E7-35F7-49D1-B02F-BFD8904E48CB}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -346,7 +346,7 @@
     Crop (arable) - plants associated with damp areas specifically</t>
       </text>
     </comment>
-    <comment ref="AO2" authorId="32" shapeId="0" xr:uid="{90E5597C-0F3C-4878-B496-32CD19452B20}">
+    <comment ref="AP2" authorId="32" shapeId="0" xr:uid="{90E5597C-0F3C-4878-B496-32CD19452B20}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -1074,24 +1074,55 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>asus:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t xml:space="preserve">
-OSR flower from April to May (early period),but ww will not. see here: http://www.fieldselection.co.uk/osr.html
-crop protection cost for OSR and ww is nearly the same (ww = £240/ha, winter OSR = £245/ha, ABC 2019)</t>
+            <color rgb="FF000000"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>asus:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">OSR flower from April to May (early period),but ww will not. see here: http://www.fieldselection.co.uk/osr.html
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>crop protection cost for OSR and ww is nearly the same (ww = £240/ha, winter OSR = £245/ha, ABC 2019)</t>
         </r>
       </text>
     </comment>
@@ -3485,7 +3516,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="244">
   <si>
     <t>hay_sil</t>
   </si>
@@ -4301,6 +4332,9 @@
   </si>
   <si>
     <t>CG_N_Snail shells</t>
+  </si>
+  <si>
+    <t>M_N_Snail shells</t>
   </si>
 </sst>
 </file>
@@ -5276,31 +5310,31 @@
   <threadedComment ref="AC2" dT="2020-06-17T10:28:36.71" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{577817A3-41CF-4B09-B701-1DA64D94A3F7}">
     <text>Margin nest</text>
   </threadedComment>
-  <threadedComment ref="AD2" dT="2020-06-17T10:27:54.75" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{61328AAB-8080-40A5-BB72-DE3F063064D6}">
+  <threadedComment ref="AE2" dT="2020-06-17T10:27:54.75" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{61328AAB-8080-40A5-BB72-DE3F063064D6}">
     <text>Crop (arable) nest</text>
   </threadedComment>
-  <threadedComment ref="AE2" dT="2020-06-17T10:28:16.09" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{08D8BC3C-7DE2-46DE-A501-79F9B77FC5A6}">
+  <threadedComment ref="AF2" dT="2020-06-17T10:28:16.09" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{08D8BC3C-7DE2-46DE-A501-79F9B77FC5A6}">
     <text>Crop (grass) nest</text>
   </threadedComment>
-  <threadedComment ref="AF2" dT="2020-06-17T10:28:18.78" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{60F49050-15F0-4A01-B60D-D08CFC1500EA}">
+  <threadedComment ref="AG2" dT="2020-06-17T10:28:18.78" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{60F49050-15F0-4A01-B60D-D08CFC1500EA}">
     <text>Crop (grass) nest</text>
   </threadedComment>
-  <threadedComment ref="AG2" dT="2020-06-17T10:28:21.43" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{53B38088-2842-4886-AD04-FB278DF6E6D5}">
+  <threadedComment ref="AH2" dT="2020-06-17T10:28:21.43" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{53B38088-2842-4886-AD04-FB278DF6E6D5}">
     <text>Crop (grass) nest</text>
   </threadedComment>
-  <threadedComment ref="AH2" dT="2020-06-17T10:28:24.74" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{E625A537-1514-4930-ADE3-685B712C12DD}">
+  <threadedComment ref="AI2" dT="2020-06-17T10:28:24.74" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{E625A537-1514-4930-ADE3-685B712C12DD}">
     <text>Crop (grass) nest</text>
   </threadedComment>
-  <threadedComment ref="AL2" dT="2020-06-17T10:30:15.35" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{2B82472E-59FF-4148-AB12-C02672624F2E}">
+  <threadedComment ref="AM2" dT="2020-06-17T10:30:15.35" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{2B82472E-59FF-4148-AB12-C02672624F2E}">
     <text>Hedge - plants associated with damp areas specifically</text>
   </threadedComment>
-  <threadedComment ref="AM2" dT="2020-06-17T10:30:22.42" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{74099FC7-8ABC-4BCA-B048-586D8C2AB079}">
+  <threadedComment ref="AN2" dT="2020-06-17T10:30:22.42" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{74099FC7-8ABC-4BCA-B048-586D8C2AB079}">
     <text>Margin - plants associated with damp areas specifically</text>
   </threadedComment>
-  <threadedComment ref="AN2" dT="2020-06-17T10:30:30.20" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{48C3A0E7-35F7-49D1-B02F-BFD8904E48CB}">
+  <threadedComment ref="AO2" dT="2020-06-17T10:30:30.20" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{48C3A0E7-35F7-49D1-B02F-BFD8904E48CB}">
     <text>Crop (arable) - plants associated with damp areas specifically</text>
   </threadedComment>
-  <threadedComment ref="AO2" dT="2020-06-17T10:30:37.43" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{90E5597C-0F3C-4878-B496-32CD19452B20}">
+  <threadedComment ref="AP2" dT="2020-06-17T10:30:37.43" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{90E5597C-0F3C-4878-B496-32CD19452B20}">
     <text>Crop (grass) - plants associated with damp areas specifically</text>
   </threadedComment>
   <threadedComment ref="E3" dT="2020-09-10T14:58:25.44" personId="{21370C70-F722-46C0-B7E0-82CA9D00A95A}" id="{C1BDF87D-1D41-44ED-9DB5-82CE7A80DFFC}">
@@ -5345,11 +5379,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64F6D29A-951C-4B7B-AAD7-CC63BC8BEE38}">
-  <dimension ref="A1:AP88"/>
+  <dimension ref="A1:AQ88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AI4" sqref="AI4"/>
+      <selection pane="bottomLeft" activeCell="AD3" sqref="AD1:AD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -5362,15 +5396,15 @@
     <col min="21" max="22" width="6.6640625" style="41" customWidth="1"/>
     <col min="23" max="23" width="3.83203125" customWidth="1"/>
     <col min="24" max="24" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="25" max="31" width="6.6640625" customWidth="1"/>
-    <col min="32" max="32" width="8.1640625" customWidth="1"/>
-    <col min="33" max="35" width="6.6640625" customWidth="1"/>
-    <col min="36" max="37" width="6.6640625" style="41" customWidth="1"/>
-    <col min="38" max="41" width="3.33203125" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="8.83203125" style="41"/>
+    <col min="25" max="32" width="6.6640625" customWidth="1"/>
+    <col min="33" max="33" width="8.1640625" customWidth="1"/>
+    <col min="34" max="36" width="6.6640625" customWidth="1"/>
+    <col min="37" max="38" width="6.6640625" style="41" customWidth="1"/>
+    <col min="39" max="42" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="8.83203125" style="41"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" s="27" customFormat="1" ht="32.75" customHeight="1">
+    <row r="1" spans="1:43" s="27" customFormat="1" ht="32.75" customHeight="1">
       <c r="A1" s="26"/>
       <c r="C1" s="76" t="s">
         <v>129</v>
@@ -5407,18 +5441,19 @@
       <c r="AF1" s="76"/>
       <c r="AG1" s="76"/>
       <c r="AH1" s="76"/>
-      <c r="AI1" s="46"/>
-      <c r="AJ1" s="47"/>
+      <c r="AI1" s="76"/>
+      <c r="AJ1" s="46"/>
       <c r="AK1" s="47"/>
-      <c r="AL1" s="77" t="s">
+      <c r="AL1" s="47"/>
+      <c r="AM1" s="77" t="s">
         <v>135</v>
       </c>
-      <c r="AM1" s="77"/>
       <c r="AN1" s="77"/>
       <c r="AO1" s="77"/>
-      <c r="AP1" s="49"/>
-    </row>
-    <row r="2" spans="1:42" s="4" customFormat="1" ht="114.5" customHeight="1">
+      <c r="AP1" s="77"/>
+      <c r="AQ1" s="49"/>
+    </row>
+    <row r="2" spans="1:43" s="4" customFormat="1" ht="114.5" customHeight="1">
       <c r="A2" s="14" t="s">
         <v>33</v>
       </c>
@@ -5506,47 +5541,50 @@
       <c r="AC2" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="AD2" s="8" t="s">
+      <c r="AD2" s="9" t="s">
+        <v>243</v>
+      </c>
+      <c r="AE2" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="AE2" s="7" t="s">
+      <c r="AF2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="AF2" s="7" t="s">
+      <c r="AG2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="AG2" s="7" t="s">
+      <c r="AH2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="AH2" s="6" t="s">
+      <c r="AI2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="AI2" s="6" t="s">
+      <c r="AJ2" s="6" t="s">
         <v>242</v>
       </c>
-      <c r="AJ2" s="48" t="s">
+      <c r="AK2" s="48" t="s">
         <v>197</v>
       </c>
-      <c r="AK2" s="48" t="s">
+      <c r="AL2" s="48" t="s">
         <v>194</v>
       </c>
-      <c r="AL2" s="5" t="s">
+      <c r="AM2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="AM2" s="5" t="s">
+      <c r="AN2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="AN2" s="5" t="s">
+      <c r="AO2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="AO2" s="5" t="s">
+      <c r="AP2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="AP2" s="50" t="s">
+      <c r="AQ2" s="50" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="3" spans="1:42" ht="16">
+    <row r="3" spans="1:43" ht="16">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -5559,7 +5597,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="4" spans="1:42" ht="16">
+    <row r="4" spans="1:43" ht="16">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -5570,11 +5608,11 @@
       <c r="F4" s="25">
         <v>-1</v>
       </c>
-      <c r="AI4" s="37">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:42" ht="16">
+      <c r="AJ4" s="37">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:43" ht="16">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -5604,7 +5642,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="6" spans="1:42" ht="16">
+    <row r="6" spans="1:43" ht="16">
       <c r="A6" s="2" t="s">
         <v>1</v>
       </c>
@@ -5621,9 +5659,6 @@
       <c r="AA6" s="37">
         <v>-1</v>
       </c>
-      <c r="AL6">
-        <v>-1</v>
-      </c>
       <c r="AM6">
         <v>-1</v>
       </c>
@@ -5633,8 +5668,11 @@
       <c r="AO6">
         <v>-1</v>
       </c>
-    </row>
-    <row r="7" spans="1:42" ht="16">
+      <c r="AP6">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:43" ht="16">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
@@ -5651,39 +5689,39 @@
       <c r="T7">
         <v>-1</v>
       </c>
-      <c r="AF7">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:42" ht="16">
+      <c r="AG7">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:43" ht="16">
       <c r="A8" s="2" t="s">
         <v>198</v>
       </c>
       <c r="F8">
         <v>-1</v>
       </c>
-      <c r="AF8">
-        <v>-1</v>
-      </c>
       <c r="AG8">
         <v>-1</v>
       </c>
-    </row>
-    <row r="9" spans="1:42">
+      <c r="AH8">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:43">
       <c r="A9" s="2"/>
     </row>
-    <row r="10" spans="1:42">
+    <row r="10" spans="1:43">
       <c r="A10" s="24"/>
       <c r="C10" s="23"/>
     </row>
-    <row r="11" spans="1:42">
+    <row r="11" spans="1:43">
       <c r="A11" s="24"/>
       <c r="C11" s="22"/>
     </row>
-    <row r="12" spans="1:42">
+    <row r="12" spans="1:43">
       <c r="A12" s="2"/>
     </row>
-    <row r="13" spans="1:42" ht="16">
+    <row r="13" spans="1:43" ht="16">
       <c r="A13" s="2" t="s">
         <v>124</v>
       </c>
@@ -5694,7 +5732,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:42" ht="16">
+    <row r="14" spans="1:43" ht="16">
       <c r="A14" s="2" t="s">
         <v>125</v>
       </c>
@@ -5705,10 +5743,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:42">
+    <row r="15" spans="1:43">
       <c r="A15" s="2"/>
     </row>
-    <row r="16" spans="1:42">
+    <row r="16" spans="1:43">
       <c r="A16" s="2"/>
     </row>
     <row r="17" spans="1:20" ht="16">
@@ -6456,8 +6494,8 @@
   <mergeCells count="4">
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="I1:T1"/>
-    <mergeCell ref="W1:AH1"/>
-    <mergeCell ref="AL1:AO1"/>
+    <mergeCell ref="W1:AI1"/>
+    <mergeCell ref="AM1:AP1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
implement analysis in black_grass_risk.R, creation of basic LMMs
</commit_message>
<xml_diff>
--- a/change.xlsx
+++ b/change.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24216"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elinfalla/Dropbox/2020-21/_Imperial_MSc/_Project/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1DF9D33-45B2-1349-8BF7-0B0E8081DDE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2531CB31-F36D-AB40-9263-7F87F780E846}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" firstSheet="7" activeTab="6" xr2:uid="{D6098C0C-5D8D-4C8C-96C7-825309F64318}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{D6098C0C-5D8D-4C8C-96C7-825309F64318}"/>
   </bookViews>
   <sheets>
-    <sheet name="pollinators" sheetId="1" r:id="rId1"/>
-    <sheet name="pollinator_key" sheetId="2" r:id="rId2"/>
+    <sheet name="bees" sheetId="1" r:id="rId1"/>
+    <sheet name="bees_key" sheetId="2" r:id="rId2"/>
     <sheet name="mammals" sheetId="3" r:id="rId3"/>
     <sheet name="mammal_key" sheetId="5" r:id="rId4"/>
     <sheet name="butterflies" sheetId="6" r:id="rId5"/>
@@ -22,7 +22,7 @@
     <sheet name="plants" sheetId="7" r:id="rId7"/>
     <sheet name="plant_key" sheetId="9" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -5507,28 +5507,28 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AD3" sqref="AD3"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3:A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8.140625" style="41" customWidth="1"/>
-    <col min="3" max="6" width="3.85546875" customWidth="1"/>
-    <col min="7" max="8" width="5.7109375" style="41" customWidth="1"/>
-    <col min="9" max="20" width="3.85546875" customWidth="1"/>
-    <col min="21" max="22" width="6.7109375" style="41" customWidth="1"/>
-    <col min="23" max="23" width="3.85546875" customWidth="1"/>
-    <col min="24" max="24" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="25" max="32" width="6.7109375" customWidth="1"/>
-    <col min="33" max="33" width="8.140625" customWidth="1"/>
-    <col min="34" max="36" width="6.7109375" customWidth="1"/>
-    <col min="37" max="38" width="6.7109375" style="41" customWidth="1"/>
-    <col min="39" max="42" width="3.28515625" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="8.85546875" style="41"/>
+    <col min="1" max="1" width="19.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8.1640625" style="41" customWidth="1"/>
+    <col min="3" max="6" width="3.83203125" customWidth="1"/>
+    <col min="7" max="8" width="5.6640625" style="41" customWidth="1"/>
+    <col min="9" max="20" width="3.83203125" customWidth="1"/>
+    <col min="21" max="22" width="6.6640625" style="41" customWidth="1"/>
+    <col min="23" max="23" width="3.83203125" customWidth="1"/>
+    <col min="24" max="24" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="32" width="6.6640625" customWidth="1"/>
+    <col min="33" max="33" width="8.1640625" customWidth="1"/>
+    <col min="34" max="36" width="6.6640625" customWidth="1"/>
+    <col min="37" max="38" width="6.6640625" style="41" customWidth="1"/>
+    <col min="39" max="42" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="8.83203125" style="41"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" s="27" customFormat="1" ht="32.85" customHeight="1">
+    <row r="1" spans="1:43" s="27" customFormat="1" ht="32.75" customHeight="1">
       <c r="A1" s="26"/>
       <c r="C1" s="84" t="s">
         <v>0</v>
@@ -5577,7 +5577,7 @@
       <c r="AP1" s="85"/>
       <c r="AQ1" s="48"/>
     </row>
-    <row r="2" spans="1:43" s="4" customFormat="1" ht="114.6" customHeight="1">
+    <row r="2" spans="1:43" s="4" customFormat="1" ht="114.5" customHeight="1">
       <c r="A2" s="14" t="s">
         <v>4</v>
       </c>
@@ -5708,7 +5708,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:43" ht="15.95">
+    <row r="3" spans="1:43" ht="16">
       <c r="A3" s="2" t="s">
         <v>47</v>
       </c>
@@ -5721,7 +5721,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="4" spans="1:43" ht="15.95">
+    <row r="4" spans="1:43" ht="16">
       <c r="A4" s="2" t="s">
         <v>48</v>
       </c>
@@ -5736,7 +5736,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="5" spans="1:43" ht="15.95">
+    <row r="5" spans="1:43" ht="16">
       <c r="A5" s="2" t="s">
         <v>49</v>
       </c>
@@ -5766,7 +5766,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="6" spans="1:43" ht="15.95">
+    <row r="6" spans="1:43" ht="16">
       <c r="A6" s="2" t="s">
         <v>50</v>
       </c>
@@ -5796,7 +5796,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="7" spans="1:43" ht="15.95">
+    <row r="7" spans="1:43" ht="16">
       <c r="A7" s="2" t="s">
         <v>51</v>
       </c>
@@ -5817,7 +5817,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="8" spans="1:43" ht="15.95">
+    <row r="8" spans="1:43" ht="16">
       <c r="A8" s="2" t="s">
         <v>52</v>
       </c>
@@ -5845,7 +5845,7 @@
     <row r="12" spans="1:43">
       <c r="A12" s="2"/>
     </row>
-    <row r="13" spans="1:43" ht="15.95">
+    <row r="13" spans="1:43" ht="16">
       <c r="A13" s="2" t="s">
         <v>53</v>
       </c>
@@ -5856,7 +5856,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:43" ht="15.95">
+    <row r="14" spans="1:43" ht="16">
       <c r="A14" s="2" t="s">
         <v>54</v>
       </c>
@@ -5873,7 +5873,7 @@
     <row r="16" spans="1:43">
       <c r="A16" s="2"/>
     </row>
-    <row r="17" spans="1:20" ht="15.95">
+    <row r="17" spans="1:20" ht="16">
       <c r="A17" s="28" t="s">
         <v>55</v>
       </c>
@@ -5885,7 +5885,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="15.95">
+    <row r="18" spans="1:20" ht="16">
       <c r="A18" s="28" t="s">
         <v>56</v>
       </c>
@@ -5914,7 +5914,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="15.95">
+    <row r="19" spans="1:20" ht="16">
       <c r="A19" s="28" t="s">
         <v>57</v>
       </c>
@@ -5926,7 +5926,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="15.95">
+    <row r="20" spans="1:20" ht="16">
       <c r="A20" s="28" t="s">
         <v>58</v>
       </c>
@@ -5955,7 +5955,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="21" spans="1:20" ht="15.95">
+    <row r="21" spans="1:20" ht="16">
       <c r="A21" s="28" t="s">
         <v>59</v>
       </c>
@@ -5967,7 +5967,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="22" spans="1:20" ht="15.95">
+    <row r="22" spans="1:20" ht="16">
       <c r="A22" s="28" t="s">
         <v>60</v>
       </c>
@@ -5996,7 +5996,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="23" spans="1:20" ht="15.95">
+    <row r="23" spans="1:20" ht="16">
       <c r="A23" s="28" t="s">
         <v>61</v>
       </c>
@@ -6008,7 +6008,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="24" spans="1:20" ht="15.95">
+    <row r="24" spans="1:20" ht="16">
       <c r="A24" s="28" t="s">
         <v>62</v>
       </c>
@@ -6037,7 +6037,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="25" spans="1:20" ht="15.95">
+    <row r="25" spans="1:20" ht="16">
       <c r="A25" s="28" t="s">
         <v>63</v>
       </c>
@@ -6049,7 +6049,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="26" spans="1:20" ht="15.95">
+    <row r="26" spans="1:20" ht="16">
       <c r="A26" s="28" t="s">
         <v>64</v>
       </c>
@@ -6078,7 +6078,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="27" spans="1:20" ht="15.95">
+    <row r="27" spans="1:20" ht="16">
       <c r="A27" s="28" t="s">
         <v>65</v>
       </c>
@@ -6090,7 +6090,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="28" spans="1:20" ht="15.95">
+    <row r="28" spans="1:20" ht="16">
       <c r="A28" s="28" t="s">
         <v>66</v>
       </c>
@@ -6125,19 +6125,19 @@
     <row r="30" spans="1:20">
       <c r="A30" s="28"/>
     </row>
-    <row r="31" spans="1:20" ht="32.1">
+    <row r="31" spans="1:20" ht="32">
       <c r="A31" s="29" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="32" spans="1:20" ht="15.95">
+    <row r="32" spans="1:20" ht="16">
       <c r="A32" s="30" t="s">
         <v>68</v>
       </c>
       <c r="E32" s="31"/>
       <c r="P32" s="31"/>
     </row>
-    <row r="33" spans="1:20" ht="15.95">
+    <row r="33" spans="1:20" ht="16">
       <c r="A33" s="30" t="s">
         <v>69</v>
       </c>
@@ -6166,14 +6166,14 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="34" spans="1:20" ht="32.1">
+    <row r="34" spans="1:20" ht="32">
       <c r="A34" s="30" t="s">
         <v>70</v>
       </c>
       <c r="E34" s="31"/>
       <c r="O34" s="31"/>
     </row>
-    <row r="35" spans="1:20" ht="32.1">
+    <row r="35" spans="1:20" ht="32">
       <c r="A35" s="30" t="s">
         <v>71</v>
       </c>
@@ -6202,7 +6202,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="36" spans="1:20" ht="15.95">
+    <row r="36" spans="1:20" ht="16">
       <c r="A36" s="30" t="s">
         <v>72</v>
       </c>
@@ -6213,7 +6213,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="37" spans="1:20" ht="15.95">
+    <row r="37" spans="1:20" ht="16">
       <c r="A37" s="30" t="s">
         <v>73</v>
       </c>
@@ -6242,7 +6242,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="38" spans="1:20" ht="15.95">
+    <row r="38" spans="1:20" ht="16">
       <c r="A38" s="30" t="s">
         <v>74</v>
       </c>
@@ -6252,12 +6252,12 @@
       <c r="A39" s="30"/>
       <c r="E39" s="31"/>
     </row>
-    <row r="40" spans="1:20" ht="15.95">
+    <row r="40" spans="1:20" ht="16">
       <c r="A40" s="30" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="41" spans="1:20" ht="15.95">
+    <row r="41" spans="1:20" ht="16">
       <c r="A41" s="30" t="s">
         <v>76</v>
       </c>
@@ -6267,14 +6267,14 @@
       </c>
       <c r="P41" s="31"/>
     </row>
-    <row r="42" spans="1:20" ht="15.95">
+    <row r="42" spans="1:20" ht="16">
       <c r="A42" s="32" t="s">
         <v>77</v>
       </c>
       <c r="E42" s="31"/>
       <c r="P42" s="31"/>
     </row>
-    <row r="43" spans="1:20" ht="15.95">
+    <row r="43" spans="1:20" ht="16">
       <c r="A43" s="30" t="s">
         <v>78</v>
       </c>
@@ -6282,7 +6282,7 @@
       <c r="O43" s="31"/>
       <c r="P43" s="31"/>
     </row>
-    <row r="44" spans="1:20" ht="15.95">
+    <row r="44" spans="1:20" ht="16">
       <c r="A44" s="30" t="s">
         <v>79</v>
       </c>
@@ -6294,14 +6294,14 @@
       </c>
       <c r="P44" s="31"/>
     </row>
-    <row r="45" spans="1:20" ht="15.95">
+    <row r="45" spans="1:20" ht="16">
       <c r="A45" s="30" t="s">
         <v>80</v>
       </c>
       <c r="E45" s="31"/>
       <c r="P45" s="31"/>
     </row>
-    <row r="46" spans="1:20" ht="14.85" customHeight="1">
+    <row r="46" spans="1:20" ht="14.75" customHeight="1">
       <c r="A46" s="30" t="s">
         <v>81</v>
       </c>
@@ -6309,7 +6309,7 @@
       <c r="O46" s="31"/>
       <c r="P46" s="31"/>
     </row>
-    <row r="47" spans="1:20" ht="15.95">
+    <row r="47" spans="1:20" ht="16">
       <c r="A47" s="30" t="s">
         <v>82</v>
       </c>
@@ -6321,19 +6321,19 @@
       </c>
       <c r="P47" s="31"/>
     </row>
-    <row r="48" spans="1:20" ht="15.95">
+    <row r="48" spans="1:20" ht="16">
       <c r="A48" s="28" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="49" spans="1:15" ht="15.95">
+    <row r="49" spans="1:15" ht="16">
       <c r="A49" s="28" t="s">
         <v>84</v>
       </c>
       <c r="E49" s="31"/>
       <c r="O49" s="31"/>
     </row>
-    <row r="50" spans="1:15" ht="15.95">
+    <row r="50" spans="1:15" ht="16">
       <c r="A50" s="28" t="s">
         <v>85</v>
       </c>
@@ -6344,19 +6344,19 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="51" spans="1:15" ht="15.95">
+    <row r="51" spans="1:15" ht="16">
       <c r="A51" s="28" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="52" spans="1:15" ht="15.95">
+    <row r="52" spans="1:15" ht="16">
       <c r="A52" s="28" t="s">
         <v>87</v>
       </c>
       <c r="E52" s="31"/>
       <c r="O52" s="31"/>
     </row>
-    <row r="53" spans="1:15" ht="15.95">
+    <row r="53" spans="1:15" ht="16">
       <c r="A53" s="28" t="s">
         <v>88</v>
       </c>
@@ -6367,17 +6367,17 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="54" spans="1:15" ht="15.95">
+    <row r="54" spans="1:15" ht="16">
       <c r="A54" s="28" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="55" spans="1:15" ht="15.95">
+    <row r="55" spans="1:15" ht="16">
       <c r="A55" s="28" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="56" spans="1:15" ht="15.95">
+    <row r="56" spans="1:15" ht="16">
       <c r="A56" s="28" t="s">
         <v>91</v>
       </c>
@@ -6388,17 +6388,17 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="57" spans="1:15" ht="15.95">
+    <row r="57" spans="1:15" ht="16">
       <c r="A57" s="28" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="58" spans="1:15" ht="15.95">
+    <row r="58" spans="1:15" ht="16">
       <c r="A58" s="28" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="59" spans="1:15" ht="15.95">
+    <row r="59" spans="1:15" ht="16">
       <c r="A59" s="28" t="s">
         <v>94</v>
       </c>
@@ -6421,26 +6421,26 @@
     <row r="63" spans="1:15">
       <c r="A63" s="28"/>
     </row>
-    <row r="64" spans="1:15" ht="32.1">
+    <row r="64" spans="1:15" ht="32">
       <c r="A64" s="29" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="65" spans="1:16" ht="15.95">
+    <row r="65" spans="1:16" ht="16">
       <c r="A65" s="30" t="s">
         <v>96</v>
       </c>
       <c r="E65" s="31"/>
       <c r="P65" s="31"/>
     </row>
-    <row r="66" spans="1:16" ht="15.95">
+    <row r="66" spans="1:16" ht="16">
       <c r="A66" s="30" t="s">
         <v>97</v>
       </c>
       <c r="E66" s="31"/>
       <c r="O66" s="31"/>
     </row>
-    <row r="67" spans="1:16" ht="15.95">
+    <row r="67" spans="1:16" ht="16">
       <c r="A67" s="30" t="s">
         <v>98</v>
       </c>
@@ -6451,18 +6451,18 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="68" spans="1:16" ht="15.95">
+    <row r="68" spans="1:16" ht="16">
       <c r="A68" s="30" t="s">
         <v>74</v>
       </c>
       <c r="E68" s="31"/>
     </row>
-    <row r="69" spans="1:16" ht="15.95">
+    <row r="69" spans="1:16" ht="16">
       <c r="A69" s="30" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="70" spans="1:16" ht="15.95">
+    <row r="70" spans="1:16" ht="16">
       <c r="A70" s="30" t="s">
         <v>76</v>
       </c>
@@ -6472,14 +6472,14 @@
       </c>
       <c r="P70" s="31"/>
     </row>
-    <row r="71" spans="1:16" ht="15.95">
+    <row r="71" spans="1:16" ht="16">
       <c r="A71" s="32" t="s">
         <v>77</v>
       </c>
       <c r="E71" s="31"/>
       <c r="P71" s="31"/>
     </row>
-    <row r="72" spans="1:16" ht="15.95">
+    <row r="72" spans="1:16" ht="16">
       <c r="A72" s="30" t="s">
         <v>78</v>
       </c>
@@ -6487,7 +6487,7 @@
       <c r="O72" s="31"/>
       <c r="P72" s="31"/>
     </row>
-    <row r="73" spans="1:16" ht="15.95">
+    <row r="73" spans="1:16" ht="16">
       <c r="A73" s="30" t="s">
         <v>79</v>
       </c>
@@ -6499,14 +6499,14 @@
       </c>
       <c r="P73" s="31"/>
     </row>
-    <row r="74" spans="1:16" ht="15.95">
+    <row r="74" spans="1:16" ht="16">
       <c r="A74" s="30" t="s">
         <v>80</v>
       </c>
       <c r="E74" s="31"/>
       <c r="P74" s="31"/>
     </row>
-    <row r="75" spans="1:16" ht="14.85" customHeight="1">
+    <row r="75" spans="1:16" ht="14.75" customHeight="1">
       <c r="A75" s="30" t="s">
         <v>81</v>
       </c>
@@ -6514,7 +6514,7 @@
       <c r="O75" s="31"/>
       <c r="P75" s="31"/>
     </row>
-    <row r="76" spans="1:16" ht="15.95">
+    <row r="76" spans="1:16" ht="16">
       <c r="A76" s="30" t="s">
         <v>82</v>
       </c>
@@ -6526,19 +6526,19 @@
       </c>
       <c r="P76" s="31"/>
     </row>
-    <row r="77" spans="1:16" ht="15.95">
+    <row r="77" spans="1:16" ht="16">
       <c r="A77" s="28" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="78" spans="1:16" ht="15.95">
+    <row r="78" spans="1:16" ht="16">
       <c r="A78" s="28" t="s">
         <v>84</v>
       </c>
       <c r="E78" s="31"/>
       <c r="O78" s="31"/>
     </row>
-    <row r="79" spans="1:16" ht="15.95">
+    <row r="79" spans="1:16" ht="16">
       <c r="A79" s="28" t="s">
         <v>85</v>
       </c>
@@ -6549,19 +6549,19 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="80" spans="1:16" ht="15.95">
+    <row r="80" spans="1:16" ht="16">
       <c r="A80" s="28" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="81" spans="1:15" ht="15.95">
+    <row r="81" spans="1:15" ht="16">
       <c r="A81" s="28" t="s">
         <v>87</v>
       </c>
       <c r="E81" s="31"/>
       <c r="O81" s="31"/>
     </row>
-    <row r="82" spans="1:15" ht="15.95">
+    <row r="82" spans="1:15" ht="16">
       <c r="A82" s="28" t="s">
         <v>88</v>
       </c>
@@ -6572,17 +6572,17 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="83" spans="1:15" ht="15.95">
+    <row r="83" spans="1:15" ht="16">
       <c r="A83" s="28" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="84" spans="1:15" ht="15.95">
+    <row r="84" spans="1:15" ht="16">
       <c r="A84" s="28" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="85" spans="1:15" ht="15.95">
+    <row r="85" spans="1:15" ht="16">
       <c r="A85" s="28" t="s">
         <v>91</v>
       </c>
@@ -6593,17 +6593,17 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="86" spans="1:15" ht="15.95">
+    <row r="86" spans="1:15" ht="16">
       <c r="A86" s="28" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="87" spans="1:15" ht="15.95">
+    <row r="87" spans="1:15" ht="16">
       <c r="A87" s="28" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="88" spans="1:15" ht="15.95">
+    <row r="88" spans="1:15" ht="16">
       <c r="A88" s="28" t="s">
         <v>94</v>
       </c>
@@ -6635,10 +6635,10 @@
       <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="26.7109375" defaultRowHeight="21" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="26.6640625" defaultRowHeight="21" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="42.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="21" customHeight="1">
@@ -7013,54 +7013,54 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B96CB725-FD77-4D87-887C-A852102D004E}">
   <dimension ref="A1:AV33"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="R1" sqref="R1:R1048576"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" style="74" customWidth="1"/>
-    <col min="3" max="4" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5" style="74" customWidth="1"/>
+    <col min="3" max="4" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="25" width="5.7109375" style="37" customWidth="1"/>
-    <col min="26" max="26" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="28" max="29" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="30" max="31" width="6.140625" style="37" customWidth="1"/>
-    <col min="32" max="32" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="8.85546875" style="37"/>
+    <col min="9" max="9" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="5.6640625" style="37" customWidth="1"/>
+    <col min="26" max="26" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="31" width="6.1640625" style="37" customWidth="1"/>
+    <col min="32" max="32" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="8.83203125" style="37"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:48" s="21" customFormat="1" ht="52.5" customHeight="1">
@@ -7209,7 +7209,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:48">
+    <row r="2" spans="1:48" ht="16">
       <c r="A2" s="2" t="s">
         <v>47</v>
       </c>
@@ -7226,7 +7226,7 @@
       </c>
       <c r="AI2" s="36"/>
     </row>
-    <row r="3" spans="1:48">
+    <row r="3" spans="1:48" ht="16">
       <c r="A3" s="2" t="s">
         <v>48</v>
       </c>
@@ -7244,7 +7244,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="4" spans="1:48" ht="30">
+    <row r="4" spans="1:48" ht="16">
       <c r="A4" s="2" t="s">
         <v>49</v>
       </c>
@@ -7283,7 +7283,7 @@
       </c>
       <c r="AU4" s="36"/>
     </row>
-    <row r="5" spans="1:48">
+    <row r="5" spans="1:48" ht="16">
       <c r="A5" s="2" t="s">
         <v>50</v>
       </c>
@@ -7318,7 +7318,7 @@
       </c>
       <c r="AU5" s="36"/>
     </row>
-    <row r="6" spans="1:48">
+    <row r="6" spans="1:48" ht="16">
       <c r="A6" s="2" t="s">
         <v>51</v>
       </c>
@@ -7330,7 +7330,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="7" spans="1:48" ht="30">
+    <row r="7" spans="1:48" ht="32">
       <c r="A7" s="2" t="s">
         <v>175</v>
       </c>
@@ -7362,7 +7362,7 @@
       <c r="A9" s="2"/>
       <c r="B9" s="24"/>
     </row>
-    <row r="10" spans="1:48">
+    <row r="10" spans="1:48" ht="16">
       <c r="A10" s="30" t="s">
         <v>176</v>
       </c>
@@ -7374,7 +7374,7 @@
       <c r="AG10" s="31"/>
       <c r="AI10" s="31"/>
     </row>
-    <row r="11" spans="1:48">
+    <row r="11" spans="1:48" ht="16">
       <c r="A11" s="30" t="s">
         <v>97</v>
       </c>
@@ -7386,7 +7386,7 @@
       <c r="AG11" s="31"/>
       <c r="AI11" s="31"/>
     </row>
-    <row r="12" spans="1:48">
+    <row r="12" spans="1:48" ht="16">
       <c r="A12" s="30" t="s">
         <v>98</v>
       </c>
@@ -7395,7 +7395,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="13" spans="1:48">
+    <row r="13" spans="1:48" ht="16">
       <c r="A13" s="30" t="s">
         <v>74</v>
       </c>
@@ -7407,13 +7407,13 @@
       <c r="AG13" s="31"/>
       <c r="AI13" s="31"/>
     </row>
-    <row r="14" spans="1:48">
+    <row r="14" spans="1:48" ht="16">
       <c r="A14" s="30" t="s">
         <v>75</v>
       </c>
       <c r="B14" s="71"/>
     </row>
-    <row r="15" spans="1:48">
+    <row r="15" spans="1:48" ht="16">
       <c r="A15" s="30" t="s">
         <v>76</v>
       </c>
@@ -7425,13 +7425,13 @@
       <c r="AG15" s="31"/>
       <c r="AI15" s="31"/>
     </row>
-    <row r="16" spans="1:48">
+    <row r="16" spans="1:48" ht="16">
       <c r="A16" s="32" t="s">
         <v>77</v>
       </c>
       <c r="B16" s="72"/>
     </row>
-    <row r="17" spans="1:35">
+    <row r="17" spans="1:35" ht="16">
       <c r="A17" s="30" t="s">
         <v>78</v>
       </c>
@@ -7443,7 +7443,7 @@
       <c r="AG17" s="31"/>
       <c r="AI17" s="31"/>
     </row>
-    <row r="18" spans="1:35">
+    <row r="18" spans="1:35" ht="16">
       <c r="A18" s="30" t="s">
         <v>79</v>
       </c>
@@ -7452,7 +7452,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="19" spans="1:35">
+    <row r="19" spans="1:35" ht="16">
       <c r="A19" s="30" t="s">
         <v>80</v>
       </c>
@@ -7462,14 +7462,14 @@
       <c r="F19" s="31"/>
       <c r="G19" s="31"/>
     </row>
-    <row r="20" spans="1:35">
+    <row r="20" spans="1:35" ht="16">
       <c r="A20" s="30" t="s">
         <v>81</v>
       </c>
       <c r="B20" s="71"/>
       <c r="E20" s="34"/>
     </row>
-    <row r="21" spans="1:35">
+    <row r="21" spans="1:35" ht="16">
       <c r="A21" s="30" t="s">
         <v>82</v>
       </c>
@@ -7478,20 +7478,20 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="22" spans="1:35">
+    <row r="22" spans="1:35" ht="16">
       <c r="A22" s="28" t="s">
         <v>83</v>
       </c>
       <c r="B22" s="73"/>
     </row>
-    <row r="23" spans="1:35">
+    <row r="23" spans="1:35" ht="16">
       <c r="A23" s="28" t="s">
         <v>84</v>
       </c>
       <c r="B23" s="73"/>
       <c r="E23" s="35"/>
     </row>
-    <row r="24" spans="1:35">
+    <row r="24" spans="1:35" ht="16">
       <c r="A24" s="28" t="s">
         <v>85</v>
       </c>
@@ -7500,20 +7500,20 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="25" spans="1:35">
+    <row r="25" spans="1:35" ht="16">
       <c r="A25" s="28" t="s">
         <v>86</v>
       </c>
       <c r="B25" s="73"/>
     </row>
-    <row r="26" spans="1:35">
+    <row r="26" spans="1:35" ht="16">
       <c r="A26" s="28" t="s">
         <v>87</v>
       </c>
       <c r="B26" s="73"/>
       <c r="E26" s="31"/>
     </row>
-    <row r="27" spans="1:35">
+    <row r="27" spans="1:35" ht="16">
       <c r="A27" s="28" t="s">
         <v>88</v>
       </c>
@@ -7522,19 +7522,19 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="28" spans="1:35" ht="30">
+    <row r="28" spans="1:35" ht="32">
       <c r="A28" s="28" t="s">
         <v>89</v>
       </c>
       <c r="B28" s="73"/>
     </row>
-    <row r="29" spans="1:35" ht="30">
+    <row r="29" spans="1:35" ht="32">
       <c r="A29" s="28" t="s">
         <v>90</v>
       </c>
       <c r="B29" s="73"/>
     </row>
-    <row r="30" spans="1:35" ht="30">
+    <row r="30" spans="1:35" ht="32">
       <c r="A30" s="28" t="s">
         <v>91</v>
       </c>
@@ -7543,19 +7543,19 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="31" spans="1:35" ht="30">
+    <row r="31" spans="1:35" ht="32">
       <c r="A31" s="28" t="s">
         <v>92</v>
       </c>
       <c r="B31" s="73"/>
     </row>
-    <row r="32" spans="1:35" ht="30">
+    <row r="32" spans="1:35" ht="32">
       <c r="A32" s="28" t="s">
         <v>93</v>
       </c>
       <c r="B32" s="73"/>
     </row>
-    <row r="33" spans="1:5" ht="30">
+    <row r="33" spans="1:5" ht="32">
       <c r="A33" s="28" t="s">
         <v>94</v>
       </c>
@@ -7579,11 +7579,11 @@
       <selection activeCell="A16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -8046,20 +8046,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39D49925-3FF0-9342-AD81-24B91F515069}">
   <dimension ref="A1:BD7"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="10.85546875" style="41"/>
-    <col min="8" max="8" width="10.85546875" style="41"/>
-    <col min="9" max="9" width="11.85546875" style="41" customWidth="1"/>
-    <col min="25" max="26" width="10.85546875" style="41"/>
-    <col min="32" max="32" width="10.85546875" style="41"/>
+    <col min="2" max="2" width="10.83203125" style="41"/>
+    <col min="8" max="8" width="10.83203125" style="41"/>
+    <col min="9" max="9" width="11.83203125" style="41" customWidth="1"/>
+    <col min="25" max="26" width="10.83203125" style="41"/>
+    <col min="32" max="32" width="10.83203125" style="41"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:56" ht="15.95">
+    <row r="1" spans="1:56" ht="16">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -8181,7 +8181,7 @@
       <c r="BC1" s="40"/>
       <c r="BD1" s="40"/>
     </row>
-    <row r="2" spans="1:56" ht="15.95">
+    <row r="2" spans="1:56" ht="16">
       <c r="A2" s="2" t="s">
         <v>47</v>
       </c>
@@ -8193,7 +8193,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="3" spans="1:56" ht="15.95">
+    <row r="3" spans="1:56" ht="16">
       <c r="A3" s="2" t="s">
         <v>48</v>
       </c>
@@ -8205,7 +8205,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="4" spans="1:56" ht="15.95">
+    <row r="4" spans="1:56" ht="16">
       <c r="A4" s="2" t="s">
         <v>49</v>
       </c>
@@ -8244,7 +8244,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="5" spans="1:56" ht="15.95">
+    <row r="5" spans="1:56" ht="16">
       <c r="A5" s="2" t="s">
         <v>50</v>
       </c>
@@ -8272,7 +8272,7 @@
       </c>
       <c r="AE5" s="37"/>
     </row>
-    <row r="6" spans="1:56" ht="15.95">
+    <row r="6" spans="1:56" ht="16">
       <c r="A6" s="2" t="s">
         <v>51</v>
       </c>
@@ -8290,7 +8290,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="7" spans="1:56" ht="15.95">
+    <row r="7" spans="1:56" ht="16">
       <c r="A7" s="2" t="s">
         <v>175</v>
       </c>
@@ -8301,6 +8301,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -8312,9 +8313,9 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="25.42578125" customWidth="1"/>
+    <col min="1" max="1" width="25.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -8325,7 +8326,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" ht="16">
       <c r="A2" s="76" t="s">
         <v>6</v>
       </c>
@@ -8333,7 +8334,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" ht="16">
       <c r="A3" s="76" t="s">
         <v>7</v>
       </c>
@@ -8341,7 +8342,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" ht="16">
       <c r="A4" s="76" t="s">
         <v>8</v>
       </c>
@@ -8349,7 +8350,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" ht="16">
       <c r="A5" s="76" t="s">
         <v>9</v>
       </c>
@@ -8357,7 +8358,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" ht="16">
       <c r="A6" s="77" t="s">
         <v>158</v>
       </c>
@@ -8365,7 +8366,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" ht="16">
       <c r="A7" s="78" t="s">
         <v>12</v>
       </c>
@@ -8373,7 +8374,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" ht="16">
       <c r="A8" s="78" t="s">
         <v>13</v>
       </c>
@@ -8381,7 +8382,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" ht="16">
       <c r="A9" s="78" t="s">
         <v>14</v>
       </c>
@@ -8389,7 +8390,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" ht="16">
       <c r="A10" s="78" t="s">
         <v>15</v>
       </c>
@@ -8397,7 +8398,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" ht="16">
       <c r="A11" s="78" t="s">
         <v>16</v>
       </c>
@@ -8405,7 +8406,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" ht="16">
       <c r="A12" s="78" t="s">
         <v>17</v>
       </c>
@@ -8413,7 +8414,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" ht="16">
       <c r="A13" s="78" t="s">
         <v>18</v>
       </c>
@@ -8421,7 +8422,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" ht="16">
       <c r="A14" s="78" t="s">
         <v>19</v>
       </c>
@@ -8429,7 +8430,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" ht="16">
       <c r="A15" s="78" t="s">
         <v>20</v>
       </c>
@@ -8437,7 +8438,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" ht="16">
       <c r="A16" s="78" t="s">
         <v>21</v>
       </c>
@@ -8445,7 +8446,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" ht="16">
       <c r="A17" s="78" t="s">
         <v>22</v>
       </c>
@@ -8453,7 +8454,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" ht="16">
       <c r="A18" s="78" t="s">
         <v>23</v>
       </c>
@@ -8461,7 +8462,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" ht="16">
       <c r="A19" s="78" t="s">
         <v>192</v>
       </c>
@@ -8469,7 +8470,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" ht="16">
       <c r="A20" s="78" t="s">
         <v>193</v>
       </c>
@@ -8477,7 +8478,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" ht="16">
       <c r="A21" s="78" t="s">
         <v>194</v>
       </c>
@@ -8485,7 +8486,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" ht="16">
       <c r="A22" s="78" t="s">
         <v>42</v>
       </c>
@@ -8493,7 +8494,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" ht="16">
       <c r="A23" s="78" t="s">
         <v>43</v>
       </c>
@@ -8501,7 +8502,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" ht="16">
       <c r="A24" s="78" t="s">
         <v>44</v>
       </c>
@@ -8509,7 +8510,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" ht="16">
       <c r="A25" s="78" t="s">
         <v>45</v>
       </c>
@@ -8517,7 +8518,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" ht="16">
       <c r="A26" s="78" t="s">
         <v>210</v>
       </c>
@@ -8534,11 +8535,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3393DC69-943B-2E4A-8022-3ED8DE99B323}">
   <dimension ref="A1:AP8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="B1:F1048576"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="U9" sqref="U9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:42">
       <c r="A1" s="50"/>
@@ -8710,7 +8711,7 @@
       <c r="AM2" s="19"/>
       <c r="AP2" s="19"/>
     </row>
-    <row r="3" spans="1:42">
+    <row r="3" spans="1:42" ht="16">
       <c r="A3" s="2" t="s">
         <v>47</v>
       </c>
@@ -8721,7 +8722,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="4" spans="1:42">
+    <row r="4" spans="1:42" ht="16">
       <c r="A4" s="2" t="s">
         <v>48</v>
       </c>
@@ -8743,7 +8744,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="5" spans="1:42">
+    <row r="5" spans="1:42" ht="16">
       <c r="A5" s="2" t="s">
         <v>49</v>
       </c>
@@ -8784,7 +8785,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="6" spans="1:42">
+    <row r="6" spans="1:42" ht="16">
       <c r="A6" s="2" t="s">
         <v>50</v>
       </c>
@@ -8816,7 +8817,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="7" spans="1:42">
+    <row r="7" spans="1:42" ht="16">
       <c r="A7" s="2" t="s">
         <v>51</v>
       </c>
@@ -8824,7 +8825,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="8" spans="1:42" ht="30">
+    <row r="8" spans="1:42" ht="16">
       <c r="A8" s="2" t="s">
         <v>175</v>
       </c>
@@ -8838,6 +8839,7 @@
     <mergeCell ref="AD1:AF1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -8850,7 +8852,7 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">

</xml_diff>